<commit_message>
final touches before finishing up !notes
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Admin" state="visible" r:id="rId4"/>
@@ -201,7 +201,7 @@
     <t>SGB</t>
   </si>
   <si>
-    <t>dklsahgdfahgjkldh</t>
+    <t>something else</t>
   </si>
   <si>
     <t>agfsdgfd</t>
@@ -1762,7 +1762,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2032,7 +2034,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="B10" sqref="B10"/>
@@ -2085,6 +2087,7 @@
         <v>55</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished !notes (I think)
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B908C459-1A6B-4349-838A-38C4D4A47202}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Admin" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Alliance" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Calendar" state="visible" r:id="rId6"/>
-    <sheet sheetId="4" name="Notes" state="visible" r:id="rId7"/>
-    <sheet sheetId="5" name="Jokes" state="visible" r:id="rId8"/>
-    <sheet sheetId="6" name="Roasts" state="visible" r:id="rId9"/>
+    <sheet name="Admin" sheetId="1" r:id="rId1"/>
+    <sheet name="Alliance" sheetId="2" r:id="rId2"/>
+    <sheet name="Calendar" sheetId="3" r:id="rId3"/>
+    <sheet name="Notes" sheetId="4" r:id="rId4"/>
+    <sheet name="Jokes" sheetId="5" r:id="rId5"/>
+    <sheet name="Roasts" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="420">
   <si>
     <t>allies</t>
   </si>
@@ -192,39 +193,6 @@
     <t>n</t>
   </si>
   <si>
-    <t>KKND</t>
-  </si>
-  <si>
-    <t>SGBR</t>
-  </si>
-  <si>
-    <t>SGB</t>
-  </si>
-  <si>
-    <t>something else</t>
-  </si>
-  <si>
-    <t>agfsdgfd</t>
-  </si>
-  <si>
-    <t>fkdl;ashjkl hjefklhagj klhhgjkreahui hjihj</t>
-  </si>
-  <si>
-    <t>something else that is new</t>
-  </si>
-  <si>
-    <t>NEW NOTE</t>
-  </si>
-  <si>
-    <t>gfsdgfdsgfsdgfsdgfds</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>this is test 2</t>
-  </si>
-  <si>
     <t>Q: What is the difference between your wife and your job?</t>
   </si>
   <si>
@@ -1353,14 +1321,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1704,51 +1672,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1759,14 +1727,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1899,14 +1867,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2033,87 +2001,40 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25"/>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B449"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F232" sqref="F232"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2121,12 +2042,12 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2134,12 +2055,12 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2147,12 +2068,12 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2160,12 +2081,12 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2173,12 +2094,12 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2186,12 +2107,12 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2199,12 +2120,12 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2212,12 +2133,12 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2225,12 +2146,12 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2238,12 +2159,12 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2251,12 +2172,12 @@
         <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2264,12 +2185,12 @@
         <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2277,12 +2198,12 @@
         <v>14</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2290,12 +2211,12 @@
         <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2303,12 +2224,12 @@
         <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2316,12 +2237,12 @@
         <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2329,12 +2250,12 @@
         <v>18</v>
       </c>
       <c r="B52" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2342,12 +2263,12 @@
         <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2355,12 +2276,12 @@
         <v>20</v>
       </c>
       <c r="B58" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2368,12 +2289,12 @@
         <v>21</v>
       </c>
       <c r="B61" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2381,12 +2302,12 @@
         <v>22</v>
       </c>
       <c r="B64" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2394,12 +2315,12 @@
         <v>23</v>
       </c>
       <c r="B67" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2407,12 +2328,12 @@
         <v>24</v>
       </c>
       <c r="B70" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2420,12 +2341,12 @@
         <v>25</v>
       </c>
       <c r="B73" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2433,12 +2354,12 @@
         <v>26</v>
       </c>
       <c r="B76" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2446,12 +2367,12 @@
         <v>27</v>
       </c>
       <c r="B79" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -2459,12 +2380,12 @@
         <v>28</v>
       </c>
       <c r="B82" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2472,12 +2393,12 @@
         <v>29</v>
       </c>
       <c r="B85" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2485,12 +2406,12 @@
         <v>30</v>
       </c>
       <c r="B88" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2498,12 +2419,12 @@
         <v>31</v>
       </c>
       <c r="B91" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2511,12 +2432,12 @@
         <v>32</v>
       </c>
       <c r="B94" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -2524,12 +2445,12 @@
         <v>33</v>
       </c>
       <c r="B97" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2537,12 +2458,12 @@
         <v>34</v>
       </c>
       <c r="B100" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2550,12 +2471,12 @@
         <v>35</v>
       </c>
       <c r="B103" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2563,12 +2484,12 @@
         <v>36</v>
       </c>
       <c r="B106" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -2576,12 +2497,12 @@
         <v>37</v>
       </c>
       <c r="B109" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -2589,12 +2510,12 @@
         <v>38</v>
       </c>
       <c r="B112" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -2602,12 +2523,12 @@
         <v>39</v>
       </c>
       <c r="B115" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -2615,12 +2536,12 @@
         <v>40</v>
       </c>
       <c r="B118" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -2628,12 +2549,12 @@
         <v>41</v>
       </c>
       <c r="B121" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -2641,12 +2562,12 @@
         <v>42</v>
       </c>
       <c r="B124" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -2654,12 +2575,12 @@
         <v>43</v>
       </c>
       <c r="B127" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -2667,12 +2588,12 @@
         <v>44</v>
       </c>
       <c r="B130" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -2680,12 +2601,12 @@
         <v>45</v>
       </c>
       <c r="B133" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -2693,12 +2614,12 @@
         <v>46</v>
       </c>
       <c r="B136" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -2706,12 +2627,12 @@
         <v>47</v>
       </c>
       <c r="B139" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -2719,12 +2640,12 @@
         <v>48</v>
       </c>
       <c r="B142" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -2732,12 +2653,12 @@
         <v>49</v>
       </c>
       <c r="B145" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -2745,12 +2666,12 @@
         <v>50</v>
       </c>
       <c r="B148" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -2758,12 +2679,12 @@
         <v>51</v>
       </c>
       <c r="B151" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -2771,12 +2692,12 @@
         <v>52</v>
       </c>
       <c r="B154" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -2784,12 +2705,12 @@
         <v>53</v>
       </c>
       <c r="B157" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -2797,12 +2718,12 @@
         <v>54</v>
       </c>
       <c r="B160" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -2810,12 +2731,12 @@
         <v>55</v>
       </c>
       <c r="B163" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -2823,12 +2744,12 @@
         <v>56</v>
       </c>
       <c r="B166" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -2836,12 +2757,12 @@
         <v>57</v>
       </c>
       <c r="B169" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -2849,12 +2770,12 @@
         <v>58</v>
       </c>
       <c r="B172" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -2862,12 +2783,12 @@
         <v>59</v>
       </c>
       <c r="B175" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -2875,12 +2796,12 @@
         <v>60</v>
       </c>
       <c r="B178" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -2888,12 +2809,12 @@
         <v>61</v>
       </c>
       <c r="B181" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -2901,12 +2822,12 @@
         <v>62</v>
       </c>
       <c r="B184" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -2914,12 +2835,12 @@
         <v>63</v>
       </c>
       <c r="B187" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -2927,12 +2848,12 @@
         <v>64</v>
       </c>
       <c r="B190" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -2940,12 +2861,12 @@
         <v>65</v>
       </c>
       <c r="B193" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -2953,12 +2874,12 @@
         <v>66</v>
       </c>
       <c r="B196" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -2966,12 +2887,12 @@
         <v>67</v>
       </c>
       <c r="B199" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -2979,12 +2900,12 @@
         <v>68</v>
       </c>
       <c r="B202" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -2992,12 +2913,12 @@
         <v>69</v>
       </c>
       <c r="B205" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
@@ -3005,12 +2926,12 @@
         <v>70</v>
       </c>
       <c r="B208" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
@@ -3018,12 +2939,12 @@
         <v>71</v>
       </c>
       <c r="B211" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
@@ -3031,12 +2952,12 @@
         <v>72</v>
       </c>
       <c r="B214" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
@@ -3044,12 +2965,12 @@
         <v>73</v>
       </c>
       <c r="B217" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
@@ -3057,12 +2978,12 @@
         <v>74</v>
       </c>
       <c r="B220" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
@@ -3070,12 +2991,12 @@
         <v>75</v>
       </c>
       <c r="B223" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
@@ -3083,12 +3004,12 @@
         <v>76</v>
       </c>
       <c r="B226" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
@@ -3096,12 +3017,12 @@
         <v>77</v>
       </c>
       <c r="B229" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
@@ -3109,12 +3030,12 @@
         <v>78</v>
       </c>
       <c r="B232" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
@@ -3122,12 +3043,12 @@
         <v>79</v>
       </c>
       <c r="B235" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
@@ -3135,12 +3056,12 @@
         <v>80</v>
       </c>
       <c r="B238" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
@@ -3148,12 +3069,12 @@
         <v>81</v>
       </c>
       <c r="B241" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
@@ -3161,12 +3082,12 @@
         <v>82</v>
       </c>
       <c r="B244" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
@@ -3174,12 +3095,12 @@
         <v>83</v>
       </c>
       <c r="B247" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
@@ -3187,12 +3108,12 @@
         <v>84</v>
       </c>
       <c r="B250" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
@@ -3200,12 +3121,12 @@
         <v>85</v>
       </c>
       <c r="B253" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
@@ -3213,12 +3134,12 @@
         <v>86</v>
       </c>
       <c r="B256" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
@@ -3226,12 +3147,12 @@
         <v>87</v>
       </c>
       <c r="B259" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
@@ -3239,12 +3160,12 @@
         <v>88</v>
       </c>
       <c r="B262" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
@@ -3252,12 +3173,12 @@
         <v>89</v>
       </c>
       <c r="B265" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="266" spans="2:2" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
@@ -3265,12 +3186,12 @@
         <v>90</v>
       </c>
       <c r="B268" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B269" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
@@ -3278,12 +3199,12 @@
         <v>91</v>
       </c>
       <c r="B271" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="272" spans="2:2" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
@@ -3291,12 +3212,12 @@
         <v>92</v>
       </c>
       <c r="B274" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B275" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
@@ -3304,12 +3225,12 @@
         <v>93</v>
       </c>
       <c r="B277" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B278" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
@@ -3317,12 +3238,12 @@
         <v>94</v>
       </c>
       <c r="B280" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="281" spans="2:2" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B281" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
@@ -3330,12 +3251,12 @@
         <v>95</v>
       </c>
       <c r="B283" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="284" spans="2:2" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B284" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
@@ -3343,12 +3264,12 @@
         <v>96</v>
       </c>
       <c r="B286" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="287" spans="2:2" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B287" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
@@ -3356,12 +3277,12 @@
         <v>97</v>
       </c>
       <c r="B289" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="290" spans="2:2" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
@@ -3369,12 +3290,12 @@
         <v>98</v>
       </c>
       <c r="B292" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="293" spans="2:2" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
@@ -3382,12 +3303,12 @@
         <v>99</v>
       </c>
       <c r="B295" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="296" spans="2:2" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B296" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
@@ -3395,12 +3316,12 @@
         <v>100</v>
       </c>
       <c r="B298" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="299" spans="2:2" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
@@ -3408,12 +3329,12 @@
         <v>101</v>
       </c>
       <c r="B301" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="302" spans="2:2" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
@@ -3421,12 +3342,12 @@
         <v>102</v>
       </c>
       <c r="B304" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="305" spans="2:2" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
@@ -3434,12 +3355,12 @@
         <v>103</v>
       </c>
       <c r="B307" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="308" spans="2:2" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
@@ -3447,12 +3368,12 @@
         <v>104</v>
       </c>
       <c r="B310" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="311" spans="2:2" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B311" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
@@ -3460,12 +3381,12 @@
         <v>105</v>
       </c>
       <c r="B313" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="314" spans="2:2" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B314" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
@@ -3473,12 +3394,12 @@
         <v>106</v>
       </c>
       <c r="B316" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="317" spans="2:2" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
@@ -3486,12 +3407,12 @@
         <v>107</v>
       </c>
       <c r="B319" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="320" spans="2:2" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B320" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
@@ -3499,12 +3420,12 @@
         <v>108</v>
       </c>
       <c r="B322" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="323" spans="2:2" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
@@ -3512,12 +3433,12 @@
         <v>109</v>
       </c>
       <c r="B325" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="326" spans="2:2" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
@@ -3525,12 +3446,12 @@
         <v>110</v>
       </c>
       <c r="B328" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="329" spans="2:2" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
@@ -3538,12 +3459,12 @@
         <v>111</v>
       </c>
       <c r="B331" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="332" spans="2:2" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
@@ -3551,12 +3472,12 @@
         <v>112</v>
       </c>
       <c r="B334" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="335" spans="2:2" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
@@ -3564,12 +3485,12 @@
         <v>113</v>
       </c>
       <c r="B337" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="338" spans="2:2" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B338" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
@@ -3577,12 +3498,12 @@
         <v>114</v>
       </c>
       <c r="B340" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="341" spans="2:2" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B341" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
@@ -3590,12 +3511,12 @@
         <v>115</v>
       </c>
       <c r="B343" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="344" spans="2:2" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B344" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
@@ -3603,12 +3524,12 @@
         <v>116</v>
       </c>
       <c r="B346" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="347" spans="2:2" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B347" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
@@ -3616,12 +3537,12 @@
         <v>117</v>
       </c>
       <c r="B349" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="350" spans="2:2" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B350" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
@@ -3629,12 +3550,12 @@
         <v>118</v>
       </c>
       <c r="B352" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="353" spans="2:2" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B353" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
@@ -3642,12 +3563,12 @@
         <v>119</v>
       </c>
       <c r="B355" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="356" spans="2:2" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B356" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
@@ -3655,12 +3576,12 @@
         <v>120</v>
       </c>
       <c r="B358" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="359" spans="2:2" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B359" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
@@ -3668,12 +3589,12 @@
         <v>121</v>
       </c>
       <c r="B361" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="362" spans="2:2" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B362" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
@@ -3681,12 +3602,12 @@
         <v>122</v>
       </c>
       <c r="B364" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="365" spans="2:2" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B365" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
@@ -3694,12 +3615,12 @@
         <v>123</v>
       </c>
       <c r="B367" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="368" spans="2:2" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B368" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
@@ -3707,12 +3628,12 @@
         <v>124</v>
       </c>
       <c r="B370" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="371" spans="2:2" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B371" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
@@ -3720,12 +3641,12 @@
         <v>125</v>
       </c>
       <c r="B373" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="374" spans="2:2" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B374" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
@@ -3733,12 +3654,12 @@
         <v>126</v>
       </c>
       <c r="B376" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="377" spans="2:2" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B377" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
@@ -3746,12 +3667,12 @@
         <v>127</v>
       </c>
       <c r="B379" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="380" spans="2:2" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B380" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
@@ -3759,12 +3680,12 @@
         <v>128</v>
       </c>
       <c r="B382" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="383" spans="2:2" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B383" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
@@ -3772,12 +3693,12 @@
         <v>129</v>
       </c>
       <c r="B385" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="386" spans="2:2" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
@@ -3785,12 +3706,12 @@
         <v>130</v>
       </c>
       <c r="B388" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="389" spans="2:2" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B389" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
@@ -3798,12 +3719,12 @@
         <v>131</v>
       </c>
       <c r="B391" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="392" spans="2:2" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B392" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
@@ -3811,12 +3732,12 @@
         <v>132</v>
       </c>
       <c r="B394" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="395" spans="2:2" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B395" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
@@ -3824,12 +3745,12 @@
         <v>133</v>
       </c>
       <c r="B397" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="398" spans="2:2" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B398" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
@@ -3837,12 +3758,12 @@
         <v>134</v>
       </c>
       <c r="B400" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="401" spans="2:2" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B401" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
@@ -3850,12 +3771,12 @@
         <v>135</v>
       </c>
       <c r="B403" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="404" spans="2:2" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B404" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
@@ -3863,12 +3784,12 @@
         <v>136</v>
       </c>
       <c r="B406" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="407" spans="2:2" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B407" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
@@ -3876,12 +3797,12 @@
         <v>137</v>
       </c>
       <c r="B409" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="410" spans="2:2" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B410" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
@@ -3889,12 +3810,12 @@
         <v>138</v>
       </c>
       <c r="B412" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="413" spans="2:2" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B413" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
@@ -3902,12 +3823,12 @@
         <v>139</v>
       </c>
       <c r="B415" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="416" spans="2:2" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B416" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
@@ -3915,12 +3836,12 @@
         <v>140</v>
       </c>
       <c r="B418" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="419" spans="2:2" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B419" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
@@ -3928,12 +3849,12 @@
         <v>141</v>
       </c>
       <c r="B421" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="422" spans="2:2" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B422" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
@@ -3941,12 +3862,12 @@
         <v>142</v>
       </c>
       <c r="B424" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="425" spans="2:2" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B425" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
@@ -3954,12 +3875,12 @@
         <v>143</v>
       </c>
       <c r="B427" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="428" spans="2:2" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B428" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
@@ -3967,12 +3888,12 @@
         <v>144</v>
       </c>
       <c r="B430" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="431" spans="2:2" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B431" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
@@ -3980,12 +3901,12 @@
         <v>145</v>
       </c>
       <c r="B433" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="434" spans="2:2" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B434" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
@@ -3993,12 +3914,12 @@
         <v>146</v>
       </c>
       <c r="B436" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="437" spans="2:2" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B437" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
@@ -4006,12 +3927,12 @@
         <v>147</v>
       </c>
       <c r="B439" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="440" spans="2:2" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B440" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
@@ -4019,12 +3940,12 @@
         <v>148</v>
       </c>
       <c r="B442" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="443" spans="2:2" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B443" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
@@ -4032,12 +3953,12 @@
         <v>149</v>
       </c>
       <c r="B445" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="446" spans="2:2" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B446" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
@@ -4045,12 +3966,12 @@
         <v>150</v>
       </c>
       <c r="B448" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
     </row>
     <row r="449" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -4059,388 +3980,388 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A75"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>410</v>
+        <v>399</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>411</v>
+        <v>400</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add !pause. New !help & !admin messages
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B908C459-1A6B-4349-838A-38C4D4A47202}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E150367-8D53-4013-A625-6FF50BC3D49A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="421">
   <si>
     <t>allies</t>
   </si>
@@ -37,51 +37,17 @@
     <t>help</t>
   </si>
   <si>
-    <t>!help: Displays this message.
-!allies: Displays the saved 'Allies' message.
-!plans: Displays the saved 'Plans' message.
-!bonus: Displays which sectors need bonus heroes.</t>
+    <t>!help - Displays this message.
+!allies - Displays info on who our current allies are in war.!plans - Gives a broad overview of our current war strategy.
+!bonus - Lists the bonus sectors that need a feature hero. (USE THIS)
+!notes - Retrieves notes on our relationships with other alliances.
+!flipacoin - Simulates a coin flip. 
+!roll - Rolls multi-sided dice. (Ex: _!roll 3d8_ rolls three, 8-sided dice)</t>
   </si>
   <si>
     <t>admin</t>
   </si>
   <si>
-    <t>!help
-    Shows basic commands
-!allies
-    Retrieves the "Allies message
-!allies set &lt;message&gt;
-    Sets the "Allies" message
-!plans
-    Retrieves the "Plans" message
-!plans set &lt;message&gt;
-    Sets the "Plans" message
-!members
-    Lists the currently saved alliance member list
-!members add &lt;member&gt;
-    Adds &lt;member&gt; to the list, up to 25
-!members remove &lt;member&gt;
-    Removes &lt;member&gt; from the list
-!bonus
-    Lists which sectors need bonus heroes and which members have their bonus hero available
-!bonus list
-    Lists currently stored bonus hero placement
-!bonus add &lt;sector&gt; &lt;member&gt;
-    Adds &lt;member&gt;'s bonus hero to &lt;sector&gt;
-!bonus remove &lt;sector&gt;
-    Searches for bonus hero on &lt;sector&gt; and clears it
-!bonus remove &lt;member&gt;
-    Searches for &lt;member&gt;'s bonus hero and clears it
-!sectors
-    Lists currently stored bonus sectors
-!sectors add &lt;sector&gt;
-    Adds &lt;sector&gt; to the list, up to 25
-!sectors remove &lt;sector&gt;
-    Removes &lt;sector&gt; from the list
-!admin
-    lists this message</t>
-  </si>
-  <si>
     <t>imothe1</t>
   </si>
   <si>
@@ -160,9 +126,6 @@
     <t>event</t>
   </si>
   <si>
-    <t>War 4</t>
-  </si>
-  <si>
     <t>War Reset</t>
   </si>
   <si>
@@ -1316,6 +1279,40 @@
   </si>
   <si>
     <t>are you always this stupid or is today a special occasion?</t>
+  </si>
+  <si>
+    <t>**!allies / !plans**
+ - These are meant to be used similar to MOTD. 
+ - Use **!allies set** and **!plans set** to record a new message. 
+ - Anyone can display that message to a channel using the command.
+**!members**
+ - Keeps track of our alliance member list (Necessary for bonus hero tracking).
+ - **!members add &lt;name&gt;** will add a new member to the list (not case sensitive).
+ - **!members remove &lt;name&gt;** will remove a member.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**!sectors**
+ - This is an admin command to keep track of which sectors we want bonus heroes on.
+ - **!sectors add &lt;sector&gt;** will add a sector to the list.
+ - Add sectors to the list as we capture new sectors that need feature heroes.
+**!sectors remove &lt;sector&gt;** removes that sector from the list.
+ - Remove sectors from the list that another alliance has captured, etc.
+**!bonus**
+ - This tracks where everyone's bonus heroes are and matches up against the sector list (described above).
+ - This is meant to quickly determine which sectors need bonus heroes.
+ - **!bonus add &lt;sector&gt; &lt;member&gt;** designates that &lt;member&gt;'s bonus hero is currently on &lt;sector&gt;.
+ - It's designed to save us the trouble of going through each sector. But we need to keep it updated to work well. I expect to do most of that legwork myself.
+ - **!bonus** will cross-check the bonus sector list (defined by !sectors) and display which sectors need bonus heroes (and who has a bonus hero available). 
+ - **!bonus remove &lt;sector or member&gt;** will search for that sector/member relationship (defined by **!bonus add**) and delete it. </t>
+  </si>
+  <si>
+    <t>**!notes**
+ - This system allows us to write and save notes on other alliances like whether we work well with them or not. 
+ - **!notes** will display a list of the alliances that we have notes for.
+ - **!notes &lt;tag&gt;** will list the notes for that particular alliance (not case sensitive).
+ - **!notes &lt;tag&gt; add &lt;message&gt;** will add your message to that alliance's note list.
+ - **!notes &lt;tag&gt; remove &lt;message&gt;** will remove a note from the list for that alliance.
+ - **!notes &lt;tag&gt; create** will add a new alliance to the list that we can add notes for.</t>
   </si>
 </sst>
 </file>
@@ -1673,10 +1670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1718,7 +1715,17 @@
     </row>
     <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -1738,127 +1745,127 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1868,7 +1875,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -1876,26 +1883,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>37</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -1906,30 +1910,24 @@
       <c r="D2">
         <v>9</v>
       </c>
-      <c r="E2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3">
-        <v>22</v>
-      </c>
-      <c r="E3">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>15</v>
@@ -1940,59 +1938,47 @@
       <c r="D4">
         <v>15</v>
       </c>
-      <c r="E4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>41</v>
       </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>42</v>
       </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2029,12 +2015,12 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2042,12 +2028,12 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2055,12 +2041,12 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2068,12 +2054,12 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2081,12 +2067,12 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2094,12 +2080,12 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2107,12 +2093,12 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2120,12 +2106,12 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2133,12 +2119,12 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2146,12 +2132,12 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2159,12 +2145,12 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2172,12 +2158,12 @@
         <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2185,12 +2171,12 @@
         <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2198,12 +2184,12 @@
         <v>14</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2211,12 +2197,12 @@
         <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2224,12 +2210,12 @@
         <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2237,12 +2223,12 @@
         <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2250,12 +2236,12 @@
         <v>18</v>
       </c>
       <c r="B52" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2263,12 +2249,12 @@
         <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2276,12 +2262,12 @@
         <v>20</v>
       </c>
       <c r="B58" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2289,12 +2275,12 @@
         <v>21</v>
       </c>
       <c r="B61" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2302,12 +2288,12 @@
         <v>22</v>
       </c>
       <c r="B64" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2315,12 +2301,12 @@
         <v>23</v>
       </c>
       <c r="B67" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2328,12 +2314,12 @@
         <v>24</v>
       </c>
       <c r="B70" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2341,12 +2327,12 @@
         <v>25</v>
       </c>
       <c r="B73" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2354,12 +2340,12 @@
         <v>26</v>
       </c>
       <c r="B76" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2367,12 +2353,12 @@
         <v>27</v>
       </c>
       <c r="B79" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -2380,12 +2366,12 @@
         <v>28</v>
       </c>
       <c r="B82" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2393,12 +2379,12 @@
         <v>29</v>
       </c>
       <c r="B85" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2406,12 +2392,12 @@
         <v>30</v>
       </c>
       <c r="B88" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2419,12 +2405,12 @@
         <v>31</v>
       </c>
       <c r="B91" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2432,12 +2418,12 @@
         <v>32</v>
       </c>
       <c r="B94" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -2445,12 +2431,12 @@
         <v>33</v>
       </c>
       <c r="B97" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2458,12 +2444,12 @@
         <v>34</v>
       </c>
       <c r="B100" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2471,12 +2457,12 @@
         <v>35</v>
       </c>
       <c r="B103" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2484,12 +2470,12 @@
         <v>36</v>
       </c>
       <c r="B106" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -2497,12 +2483,12 @@
         <v>37</v>
       </c>
       <c r="B109" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -2510,12 +2496,12 @@
         <v>38</v>
       </c>
       <c r="B112" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -2523,12 +2509,12 @@
         <v>39</v>
       </c>
       <c r="B115" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -2536,12 +2522,12 @@
         <v>40</v>
       </c>
       <c r="B118" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -2549,12 +2535,12 @@
         <v>41</v>
       </c>
       <c r="B121" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -2562,12 +2548,12 @@
         <v>42</v>
       </c>
       <c r="B124" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -2575,12 +2561,12 @@
         <v>43</v>
       </c>
       <c r="B127" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -2588,12 +2574,12 @@
         <v>44</v>
       </c>
       <c r="B130" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -2601,12 +2587,12 @@
         <v>45</v>
       </c>
       <c r="B133" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -2614,12 +2600,12 @@
         <v>46</v>
       </c>
       <c r="B136" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -2627,12 +2613,12 @@
         <v>47</v>
       </c>
       <c r="B139" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -2640,12 +2626,12 @@
         <v>48</v>
       </c>
       <c r="B142" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -2653,12 +2639,12 @@
         <v>49</v>
       </c>
       <c r="B145" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -2666,12 +2652,12 @@
         <v>50</v>
       </c>
       <c r="B148" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -2679,12 +2665,12 @@
         <v>51</v>
       </c>
       <c r="B151" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -2692,12 +2678,12 @@
         <v>52</v>
       </c>
       <c r="B154" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -2705,12 +2691,12 @@
         <v>53</v>
       </c>
       <c r="B157" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -2718,12 +2704,12 @@
         <v>54</v>
       </c>
       <c r="B160" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -2731,12 +2717,12 @@
         <v>55</v>
       </c>
       <c r="B163" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -2744,12 +2730,12 @@
         <v>56</v>
       </c>
       <c r="B166" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -2757,12 +2743,12 @@
         <v>57</v>
       </c>
       <c r="B169" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -2770,12 +2756,12 @@
         <v>58</v>
       </c>
       <c r="B172" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -2783,12 +2769,12 @@
         <v>59</v>
       </c>
       <c r="B175" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -2796,12 +2782,12 @@
         <v>60</v>
       </c>
       <c r="B178" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -2809,12 +2795,12 @@
         <v>61</v>
       </c>
       <c r="B181" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -2822,12 +2808,12 @@
         <v>62</v>
       </c>
       <c r="B184" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -2835,12 +2821,12 @@
         <v>63</v>
       </c>
       <c r="B187" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -2848,12 +2834,12 @@
         <v>64</v>
       </c>
       <c r="B190" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -2861,12 +2847,12 @@
         <v>65</v>
       </c>
       <c r="B193" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -2874,12 +2860,12 @@
         <v>66</v>
       </c>
       <c r="B196" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -2887,12 +2873,12 @@
         <v>67</v>
       </c>
       <c r="B199" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -2900,12 +2886,12 @@
         <v>68</v>
       </c>
       <c r="B202" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -2913,12 +2899,12 @@
         <v>69</v>
       </c>
       <c r="B205" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
@@ -2926,12 +2912,12 @@
         <v>70</v>
       </c>
       <c r="B208" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
@@ -2939,12 +2925,12 @@
         <v>71</v>
       </c>
       <c r="B211" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
@@ -2952,12 +2938,12 @@
         <v>72</v>
       </c>
       <c r="B214" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
@@ -2965,12 +2951,12 @@
         <v>73</v>
       </c>
       <c r="B217" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
@@ -2978,12 +2964,12 @@
         <v>74</v>
       </c>
       <c r="B220" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
@@ -2991,12 +2977,12 @@
         <v>75</v>
       </c>
       <c r="B223" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
@@ -3004,12 +2990,12 @@
         <v>76</v>
       </c>
       <c r="B226" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
@@ -3017,12 +3003,12 @@
         <v>77</v>
       </c>
       <c r="B229" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
@@ -3030,12 +3016,12 @@
         <v>78</v>
       </c>
       <c r="B232" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
@@ -3043,12 +3029,12 @@
         <v>79</v>
       </c>
       <c r="B235" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
@@ -3056,12 +3042,12 @@
         <v>80</v>
       </c>
       <c r="B238" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
@@ -3069,12 +3055,12 @@
         <v>81</v>
       </c>
       <c r="B241" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
@@ -3082,12 +3068,12 @@
         <v>82</v>
       </c>
       <c r="B244" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
@@ -3095,12 +3081,12 @@
         <v>83</v>
       </c>
       <c r="B247" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
@@ -3108,12 +3094,12 @@
         <v>84</v>
       </c>
       <c r="B250" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
@@ -3121,12 +3107,12 @@
         <v>85</v>
       </c>
       <c r="B253" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
@@ -3134,12 +3120,12 @@
         <v>86</v>
       </c>
       <c r="B256" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
@@ -3147,12 +3133,12 @@
         <v>87</v>
       </c>
       <c r="B259" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
@@ -3160,12 +3146,12 @@
         <v>88</v>
       </c>
       <c r="B262" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
@@ -3173,12 +3159,12 @@
         <v>89</v>
       </c>
       <c r="B265" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
@@ -3186,12 +3172,12 @@
         <v>90</v>
       </c>
       <c r="B268" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B269" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
@@ -3199,12 +3185,12 @@
         <v>91</v>
       </c>
       <c r="B271" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
@@ -3212,12 +3198,12 @@
         <v>92</v>
       </c>
       <c r="B274" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B275" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
@@ -3225,12 +3211,12 @@
         <v>93</v>
       </c>
       <c r="B277" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B278" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
@@ -3238,12 +3224,12 @@
         <v>94</v>
       </c>
       <c r="B280" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B281" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
@@ -3251,12 +3237,12 @@
         <v>95</v>
       </c>
       <c r="B283" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B284" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
@@ -3264,12 +3250,12 @@
         <v>96</v>
       </c>
       <c r="B286" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B287" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
@@ -3277,12 +3263,12 @@
         <v>97</v>
       </c>
       <c r="B289" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
@@ -3290,12 +3276,12 @@
         <v>98</v>
       </c>
       <c r="B292" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
@@ -3303,12 +3289,12 @@
         <v>99</v>
       </c>
       <c r="B295" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B296" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
@@ -3316,12 +3302,12 @@
         <v>100</v>
       </c>
       <c r="B298" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
@@ -3329,12 +3315,12 @@
         <v>101</v>
       </c>
       <c r="B301" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
@@ -3342,12 +3328,12 @@
         <v>102</v>
       </c>
       <c r="B304" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
@@ -3355,12 +3341,12 @@
         <v>103</v>
       </c>
       <c r="B307" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
@@ -3368,12 +3354,12 @@
         <v>104</v>
       </c>
       <c r="B310" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B311" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
@@ -3381,12 +3367,12 @@
         <v>105</v>
       </c>
       <c r="B313" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B314" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
@@ -3394,12 +3380,12 @@
         <v>106</v>
       </c>
       <c r="B316" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
@@ -3407,12 +3393,12 @@
         <v>107</v>
       </c>
       <c r="B319" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B320" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
@@ -3420,12 +3406,12 @@
         <v>108</v>
       </c>
       <c r="B322" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
@@ -3433,12 +3419,12 @@
         <v>109</v>
       </c>
       <c r="B325" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
@@ -3446,12 +3432,12 @@
         <v>110</v>
       </c>
       <c r="B328" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
@@ -3459,12 +3445,12 @@
         <v>111</v>
       </c>
       <c r="B331" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
@@ -3472,12 +3458,12 @@
         <v>112</v>
       </c>
       <c r="B334" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
@@ -3485,12 +3471,12 @@
         <v>113</v>
       </c>
       <c r="B337" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B338" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
@@ -3498,12 +3484,12 @@
         <v>114</v>
       </c>
       <c r="B340" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B341" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
@@ -3511,12 +3497,12 @@
         <v>115</v>
       </c>
       <c r="B343" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B344" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
@@ -3524,12 +3510,12 @@
         <v>116</v>
       </c>
       <c r="B346" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B347" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
@@ -3537,12 +3523,12 @@
         <v>117</v>
       </c>
       <c r="B349" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B350" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
@@ -3550,12 +3536,12 @@
         <v>118</v>
       </c>
       <c r="B352" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B353" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
@@ -3563,12 +3549,12 @@
         <v>119</v>
       </c>
       <c r="B355" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B356" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
@@ -3576,12 +3562,12 @@
         <v>120</v>
       </c>
       <c r="B358" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B359" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
@@ -3589,12 +3575,12 @@
         <v>121</v>
       </c>
       <c r="B361" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B362" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
@@ -3602,12 +3588,12 @@
         <v>122</v>
       </c>
       <c r="B364" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B365" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
@@ -3615,12 +3601,12 @@
         <v>123</v>
       </c>
       <c r="B367" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B368" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
@@ -3628,12 +3614,12 @@
         <v>124</v>
       </c>
       <c r="B370" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B371" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
@@ -3641,12 +3627,12 @@
         <v>125</v>
       </c>
       <c r="B373" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B374" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
@@ -3654,12 +3640,12 @@
         <v>126</v>
       </c>
       <c r="B376" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B377" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
@@ -3667,12 +3653,12 @@
         <v>127</v>
       </c>
       <c r="B379" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B380" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
@@ -3680,12 +3666,12 @@
         <v>128</v>
       </c>
       <c r="B382" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B383" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
@@ -3693,12 +3679,12 @@
         <v>129</v>
       </c>
       <c r="B385" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
@@ -3706,12 +3692,12 @@
         <v>130</v>
       </c>
       <c r="B388" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B389" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
@@ -3719,12 +3705,12 @@
         <v>131</v>
       </c>
       <c r="B391" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B392" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
@@ -3732,12 +3718,12 @@
         <v>132</v>
       </c>
       <c r="B394" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B395" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
@@ -3745,12 +3731,12 @@
         <v>133</v>
       </c>
       <c r="B397" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B398" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
@@ -3758,12 +3744,12 @@
         <v>134</v>
       </c>
       <c r="B400" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B401" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
@@ -3771,12 +3757,12 @@
         <v>135</v>
       </c>
       <c r="B403" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B404" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
@@ -3784,12 +3770,12 @@
         <v>136</v>
       </c>
       <c r="B406" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B407" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
@@ -3797,12 +3783,12 @@
         <v>137</v>
       </c>
       <c r="B409" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B410" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
@@ -3810,12 +3796,12 @@
         <v>138</v>
       </c>
       <c r="B412" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B413" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
@@ -3823,12 +3809,12 @@
         <v>139</v>
       </c>
       <c r="B415" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B416" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
@@ -3836,12 +3822,12 @@
         <v>140</v>
       </c>
       <c r="B418" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B419" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
@@ -3849,12 +3835,12 @@
         <v>141</v>
       </c>
       <c r="B421" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B422" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
@@ -3862,12 +3848,12 @@
         <v>142</v>
       </c>
       <c r="B424" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B425" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
@@ -3875,12 +3861,12 @@
         <v>143</v>
       </c>
       <c r="B427" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B428" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
@@ -3888,12 +3874,12 @@
         <v>144</v>
       </c>
       <c r="B430" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B431" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
@@ -3901,12 +3887,12 @@
         <v>145</v>
       </c>
       <c r="B433" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B434" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
@@ -3914,12 +3900,12 @@
         <v>146</v>
       </c>
       <c r="B436" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B437" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
@@ -3927,12 +3913,12 @@
         <v>147</v>
       </c>
       <c r="B439" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B440" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
@@ -3940,12 +3926,12 @@
         <v>148</v>
       </c>
       <c r="B442" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B443" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
@@ -3953,12 +3939,12 @@
         <v>149</v>
       </c>
       <c r="B445" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B446" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
@@ -3966,12 +3952,12 @@
         <v>150</v>
       </c>
       <c r="B448" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="449" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -3991,377 +3977,377 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
!bonus add/remove with partial strings
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="446">
   <si>
     <t>allies</t>
   </si>
@@ -37,7 +37,8 @@
   </si>
   <si>
     <t>!help - Displays this message.
-!allies - Displays info on who our current allies are in war.!plans - Gives a broad overview of our current war strategy.
+!allies - Displays info on who our current allies are in war.
+!plans - Gives a broad overview of our current war strategy.
 !bonus - Lists the bonus sectors that need a feature hero. (USE THIS)
 !notes - Retrieves notes on our relationships with other alliances.
 !flipacoin - Simulates a coin flip. 
@@ -47,7 +48,8 @@
     <t>admin</t>
   </si>
   <si>
-    <t>_**!allies / !plans**
+    <t>_
+**!allies / !plans**
  - These are meant to be used similar to MOTD. 
  - Use **!allies set** and **!plans set** to record a new message. 
  - Anyone can display that message to a channel using the command.</t>
@@ -76,6 +78,7 @@
  - **!bonus add &lt;sector&gt; &lt;member&gt;** designates that &lt;member&gt;'s bonus hero is currently on &lt;sector&gt;.
  - It's designed to save us the trouble of going through each sector. But we need to keep it updated to work well. I expect to do most of that legwork myself.
  - **!bonus** will cross-check the bonus sector list (defined by !sectors) and display which sectors need bonus heroes (and who has a bonus hero available). 
+ - **!bonus list** will display every alliance member and their bonus hero placement (if recorded).
  - **!bonus remove &lt;sector or member&gt;** will search for that sector/member relationship (defined by **!bonus add**) and delete it. </t>
   </si>
   <si>
@@ -101,93 +104,99 @@
     <t>xmousecop</t>
   </si>
   <si>
+    <t>217</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>wrathavenger</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>teamgb</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>shooty pants</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>sarcasticahole</t>
+  </si>
+  <si>
+    <t>204</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>ru1900</t>
+  </si>
+  <si>
+    <t>216</t>
+  </si>
+  <si>
+    <t>rickys ruff riders</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
+    <t>2inpink 3instink</t>
+  </si>
+  <si>
+    <t>pratt11</t>
+  </si>
+  <si>
+    <t>165</t>
+  </si>
+  <si>
+    <t>peekaboo123</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>papa marsh</t>
+  </si>
+  <si>
+    <t>199</t>
+  </si>
+  <si>
+    <t>ocivv</t>
+  </si>
+  <si>
+    <t>nae blis</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>117</t>
-  </si>
-  <si>
-    <t>wrathavenger</t>
-  </si>
-  <si>
-    <t>118</t>
-  </si>
-  <si>
-    <t>teamgb</t>
-  </si>
-  <si>
-    <t>140</t>
-  </si>
-  <si>
-    <t>121</t>
-  </si>
-  <si>
-    <t>shooty pants</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>sarcasticahole</t>
-  </si>
-  <si>
-    <t>139</t>
-  </si>
-  <si>
-    <t>ru1900</t>
-  </si>
-  <si>
-    <t>rickys ruff riders</t>
-  </si>
-  <si>
-    <t>159</t>
-  </si>
-  <si>
-    <t>2inpink 3instink</t>
-  </si>
-  <si>
-    <t>pratt11</t>
-  </si>
-  <si>
-    <t>165</t>
-  </si>
-  <si>
-    <t>peekaboo123</t>
-  </si>
-  <si>
-    <t>177</t>
-  </si>
-  <si>
-    <t>papa marsh</t>
-  </si>
-  <si>
-    <t>199</t>
-  </si>
-  <si>
-    <t>178</t>
-  </si>
-  <si>
-    <t>ocivv</t>
-  </si>
-  <si>
-    <t>nae blis</t>
-  </si>
-  <si>
     <t>202</t>
   </si>
   <si>
     <t>msbatman</t>
   </si>
   <si>
-    <t>204</t>
+    <t>203</t>
   </si>
   <si>
     <t>boricua</t>
   </si>
   <si>
-    <t>217</t>
-  </si>
-  <si>
     <t>korvvish</t>
   </si>
   <si>
@@ -197,6 +206,9 @@
     <t>kashmeoutside</t>
   </si>
   <si>
+    <t>182</t>
+  </si>
+  <si>
     <t>198</t>
   </si>
   <si>
@@ -204,6 +216,9 @@
   </si>
   <si>
     <t>i n0mad i</t>
+  </si>
+  <si>
+    <t>218</t>
   </si>
   <si>
     <t>dracolatias</t>
@@ -1737,7 +1752,7 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" customHeight="1"/>
@@ -1843,59 +1858,71 @@
       <c r="A3" t="s">
         <v>18</v>
       </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
@@ -1903,139 +1930,154 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2055,21 +2097,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -2083,7 +2125,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B3">
         <v>21</v>
@@ -2097,7 +2139,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B4">
         <v>15</v>
@@ -2111,44 +2153,44 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2185,12 +2227,12 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2198,12 +2240,12 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2211,12 +2253,12 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2224,12 +2266,12 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2237,12 +2279,12 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2250,12 +2292,12 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2263,12 +2305,12 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2276,12 +2318,12 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2289,12 +2331,12 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2302,12 +2344,12 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2315,12 +2357,12 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2328,12 +2370,12 @@
         <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2341,12 +2383,12 @@
         <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2354,12 +2396,12 @@
         <v>14</v>
       </c>
       <c r="B40" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2367,12 +2409,12 @@
         <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2380,12 +2422,12 @@
         <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2393,12 +2435,12 @@
         <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2406,12 +2448,12 @@
         <v>18</v>
       </c>
       <c r="B52" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2419,12 +2461,12 @@
         <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2432,12 +2474,12 @@
         <v>20</v>
       </c>
       <c r="B58" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2445,12 +2487,12 @@
         <v>21</v>
       </c>
       <c r="B61" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2458,12 +2500,12 @@
         <v>22</v>
       </c>
       <c r="B64" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2471,12 +2513,12 @@
         <v>23</v>
       </c>
       <c r="B67" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2484,12 +2526,12 @@
         <v>24</v>
       </c>
       <c r="B70" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2497,12 +2539,12 @@
         <v>25</v>
       </c>
       <c r="B73" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2510,12 +2552,12 @@
         <v>26</v>
       </c>
       <c r="B76" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2523,12 +2565,12 @@
         <v>27</v>
       </c>
       <c r="B79" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -2536,12 +2578,12 @@
         <v>28</v>
       </c>
       <c r="B82" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2549,12 +2591,12 @@
         <v>29</v>
       </c>
       <c r="B85" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2562,12 +2604,12 @@
         <v>30</v>
       </c>
       <c r="B88" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2575,12 +2617,12 @@
         <v>31</v>
       </c>
       <c r="B91" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2588,12 +2630,12 @@
         <v>32</v>
       </c>
       <c r="B94" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -2601,12 +2643,12 @@
         <v>33</v>
       </c>
       <c r="B97" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2614,12 +2656,12 @@
         <v>34</v>
       </c>
       <c r="B100" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2627,12 +2669,12 @@
         <v>35</v>
       </c>
       <c r="B103" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2640,12 +2682,12 @@
         <v>36</v>
       </c>
       <c r="B106" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -2653,12 +2695,12 @@
         <v>37</v>
       </c>
       <c r="B109" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -2666,12 +2708,12 @@
         <v>38</v>
       </c>
       <c r="B112" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -2679,12 +2721,12 @@
         <v>39</v>
       </c>
       <c r="B115" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -2692,12 +2734,12 @@
         <v>40</v>
       </c>
       <c r="B118" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -2705,12 +2747,12 @@
         <v>41</v>
       </c>
       <c r="B121" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -2718,12 +2760,12 @@
         <v>42</v>
       </c>
       <c r="B124" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -2731,12 +2773,12 @@
         <v>43</v>
       </c>
       <c r="B127" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -2744,12 +2786,12 @@
         <v>44</v>
       </c>
       <c r="B130" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -2757,12 +2799,12 @@
         <v>45</v>
       </c>
       <c r="B133" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -2770,12 +2812,12 @@
         <v>46</v>
       </c>
       <c r="B136" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -2783,12 +2825,12 @@
         <v>47</v>
       </c>
       <c r="B139" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -2796,12 +2838,12 @@
         <v>48</v>
       </c>
       <c r="B142" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -2809,12 +2851,12 @@
         <v>49</v>
       </c>
       <c r="B145" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -2822,12 +2864,12 @@
         <v>50</v>
       </c>
       <c r="B148" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -2835,12 +2877,12 @@
         <v>51</v>
       </c>
       <c r="B151" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -2848,12 +2890,12 @@
         <v>52</v>
       </c>
       <c r="B154" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -2861,12 +2903,12 @@
         <v>53</v>
       </c>
       <c r="B157" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -2874,12 +2916,12 @@
         <v>54</v>
       </c>
       <c r="B160" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -2887,12 +2929,12 @@
         <v>55</v>
       </c>
       <c r="B163" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -2900,12 +2942,12 @@
         <v>56</v>
       </c>
       <c r="B166" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -2913,12 +2955,12 @@
         <v>57</v>
       </c>
       <c r="B169" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -2926,12 +2968,12 @@
         <v>58</v>
       </c>
       <c r="B172" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -2939,12 +2981,12 @@
         <v>59</v>
       </c>
       <c r="B175" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -2952,12 +2994,12 @@
         <v>60</v>
       </c>
       <c r="B178" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="179" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -2965,12 +3007,12 @@
         <v>61</v>
       </c>
       <c r="B181" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="182" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -2978,12 +3020,12 @@
         <v>62</v>
       </c>
       <c r="B184" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="185" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -2991,12 +3033,12 @@
         <v>63</v>
       </c>
       <c r="B187" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="188" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -3004,12 +3046,12 @@
         <v>64</v>
       </c>
       <c r="B190" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="191" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -3017,12 +3059,12 @@
         <v>65</v>
       </c>
       <c r="B193" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="194" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -3030,12 +3072,12 @@
         <v>66</v>
       </c>
       <c r="B196" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="197" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -3043,12 +3085,12 @@
         <v>67</v>
       </c>
       <c r="B199" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="200" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -3056,12 +3098,12 @@
         <v>68</v>
       </c>
       <c r="B202" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="203" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -3069,12 +3111,12 @@
         <v>69</v>
       </c>
       <c r="B205" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="206" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
@@ -3082,12 +3124,12 @@
         <v>70</v>
       </c>
       <c r="B208" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
@@ -3095,12 +3137,12 @@
         <v>71</v>
       </c>
       <c r="B211" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="212" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
@@ -3108,12 +3150,12 @@
         <v>72</v>
       </c>
       <c r="B214" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="215" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
@@ -3121,12 +3163,12 @@
         <v>73</v>
       </c>
       <c r="B217" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="218" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
@@ -3134,12 +3176,12 @@
         <v>74</v>
       </c>
       <c r="B220" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="221" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
@@ -3147,12 +3189,12 @@
         <v>75</v>
       </c>
       <c r="B223" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="224" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
@@ -3160,12 +3202,12 @@
         <v>76</v>
       </c>
       <c r="B226" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="227" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
@@ -3173,12 +3215,12 @@
         <v>77</v>
       </c>
       <c r="B229" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="230" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
@@ -3186,12 +3228,12 @@
         <v>78</v>
       </c>
       <c r="B232" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="233" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
@@ -3199,12 +3241,12 @@
         <v>79</v>
       </c>
       <c r="B235" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="236" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
@@ -3212,12 +3254,12 @@
         <v>80</v>
       </c>
       <c r="B238" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="239" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
@@ -3225,12 +3267,12 @@
         <v>81</v>
       </c>
       <c r="B241" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="242" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
@@ -3238,12 +3280,12 @@
         <v>82</v>
       </c>
       <c r="B244" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="245" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
@@ -3251,12 +3293,12 @@
         <v>83</v>
       </c>
       <c r="B247" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="248" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
@@ -3264,12 +3306,12 @@
         <v>84</v>
       </c>
       <c r="B250" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="251" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
@@ -3277,12 +3319,12 @@
         <v>85</v>
       </c>
       <c r="B253" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="254" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
@@ -3290,12 +3332,12 @@
         <v>86</v>
       </c>
       <c r="B256" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="257" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
@@ -3303,12 +3345,12 @@
         <v>87</v>
       </c>
       <c r="B259" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="260" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
@@ -3316,12 +3358,12 @@
         <v>88</v>
       </c>
       <c r="B262" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="263" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
@@ -3329,12 +3371,12 @@
         <v>89</v>
       </c>
       <c r="B265" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="266" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
@@ -3342,12 +3384,12 @@
         <v>90</v>
       </c>
       <c r="B268" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="269" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B269" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
@@ -3355,12 +3397,12 @@
         <v>91</v>
       </c>
       <c r="B271" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="272" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
@@ -3368,12 +3410,12 @@
         <v>92</v>
       </c>
       <c r="B274" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="275" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B275" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
@@ -3381,12 +3423,12 @@
         <v>93</v>
       </c>
       <c r="B277" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="278" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B278" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
@@ -3394,12 +3436,12 @@
         <v>94</v>
       </c>
       <c r="B280" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="281" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B281" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
@@ -3407,12 +3449,12 @@
         <v>95</v>
       </c>
       <c r="B283" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="284" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B284" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
@@ -3420,12 +3462,12 @@
         <v>96</v>
       </c>
       <c r="B286" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="287" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B287" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
@@ -3433,12 +3475,12 @@
         <v>97</v>
       </c>
       <c r="B289" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="290" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
@@ -3446,12 +3488,12 @@
         <v>98</v>
       </c>
       <c r="B292" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="293" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
@@ -3459,12 +3501,12 @@
         <v>99</v>
       </c>
       <c r="B295" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="296" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B296" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
@@ -3472,12 +3514,12 @@
         <v>100</v>
       </c>
       <c r="B298" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="299" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
@@ -3485,12 +3527,12 @@
         <v>101</v>
       </c>
       <c r="B301" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="302" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
@@ -3498,12 +3540,12 @@
         <v>102</v>
       </c>
       <c r="B304" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="305" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
@@ -3511,12 +3553,12 @@
         <v>103</v>
       </c>
       <c r="B307" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="308" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
@@ -3524,12 +3566,12 @@
         <v>104</v>
       </c>
       <c r="B310" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="311" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B311" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
@@ -3537,12 +3579,12 @@
         <v>105</v>
       </c>
       <c r="B313" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="314" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B314" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
@@ -3550,12 +3592,12 @@
         <v>106</v>
       </c>
       <c r="B316" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="317" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
@@ -3563,12 +3605,12 @@
         <v>107</v>
       </c>
       <c r="B319" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="320" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B320" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
@@ -3576,12 +3618,12 @@
         <v>108</v>
       </c>
       <c r="B322" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="323" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
@@ -3589,12 +3631,12 @@
         <v>109</v>
       </c>
       <c r="B325" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="326" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
@@ -3602,12 +3644,12 @@
         <v>110</v>
       </c>
       <c r="B328" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="329" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
@@ -3615,12 +3657,12 @@
         <v>111</v>
       </c>
       <c r="B331" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="332" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
@@ -3628,12 +3670,12 @@
         <v>112</v>
       </c>
       <c r="B334" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="335" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
@@ -3641,12 +3683,12 @@
         <v>113</v>
       </c>
       <c r="B337" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="338" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B338" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
@@ -3654,12 +3696,12 @@
         <v>114</v>
       </c>
       <c r="B340" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="341" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B341" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
@@ -3667,12 +3709,12 @@
         <v>115</v>
       </c>
       <c r="B343" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
     <row r="344" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B344" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
@@ -3680,12 +3722,12 @@
         <v>116</v>
       </c>
       <c r="B346" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
     </row>
     <row r="347" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B347" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
@@ -3693,12 +3735,12 @@
         <v>117</v>
       </c>
       <c r="B349" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
     </row>
     <row r="350" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B350" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
@@ -3706,12 +3748,12 @@
         <v>118</v>
       </c>
       <c r="B352" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="353" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B353" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
@@ -3719,12 +3761,12 @@
         <v>119</v>
       </c>
       <c r="B355" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
     </row>
     <row r="356" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B356" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
@@ -3732,12 +3774,12 @@
         <v>120</v>
       </c>
       <c r="B358" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="359" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B359" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
@@ -3745,12 +3787,12 @@
         <v>121</v>
       </c>
       <c r="B361" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="362" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B362" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
@@ -3758,12 +3800,12 @@
         <v>122</v>
       </c>
       <c r="B364" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
     <row r="365" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B365" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
@@ -3771,12 +3813,12 @@
         <v>123</v>
       </c>
       <c r="B367" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="368" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B368" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
@@ -3784,12 +3826,12 @@
         <v>124</v>
       </c>
       <c r="B370" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="371" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B371" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
@@ -3797,12 +3839,12 @@
         <v>125</v>
       </c>
       <c r="B373" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="374" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B374" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
@@ -3810,12 +3852,12 @@
         <v>126</v>
       </c>
       <c r="B376" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="377" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B377" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
@@ -3823,12 +3865,12 @@
         <v>127</v>
       </c>
       <c r="B379" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
     <row r="380" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B380" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
@@ -3836,12 +3878,12 @@
         <v>128</v>
       </c>
       <c r="B382" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="383" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B383" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
@@ -3849,12 +3891,12 @@
         <v>129</v>
       </c>
       <c r="B385" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
     <row r="386" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
@@ -3862,12 +3904,12 @@
         <v>130</v>
       </c>
       <c r="B388" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="389" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B389" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
@@ -3875,12 +3917,12 @@
         <v>131</v>
       </c>
       <c r="B391" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="392" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B392" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
@@ -3888,12 +3930,12 @@
         <v>132</v>
       </c>
       <c r="B394" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row r="395" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B395" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
@@ -3901,12 +3943,12 @@
         <v>133</v>
       </c>
       <c r="B397" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="398" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B398" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
@@ -3914,12 +3956,12 @@
         <v>134</v>
       </c>
       <c r="B400" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
     <row r="401" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B401" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
@@ -3927,12 +3969,12 @@
         <v>135</v>
       </c>
       <c r="B403" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
     </row>
     <row r="404" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B404" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
@@ -3940,12 +3982,12 @@
         <v>136</v>
       </c>
       <c r="B406" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
     </row>
     <row r="407" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B407" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
@@ -3953,12 +3995,12 @@
         <v>137</v>
       </c>
       <c r="B409" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="410" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B410" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
@@ -3966,12 +4008,12 @@
         <v>138</v>
       </c>
       <c r="B412" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
     </row>
     <row r="413" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B413" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
@@ -3979,12 +4021,12 @@
         <v>139</v>
       </c>
       <c r="B415" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row r="416" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B416" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
@@ -3992,12 +4034,12 @@
         <v>140</v>
       </c>
       <c r="B418" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
     </row>
     <row r="419" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B419" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
@@ -4005,12 +4047,12 @@
         <v>141</v>
       </c>
       <c r="B421" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="422" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B422" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
@@ -4018,12 +4060,12 @@
         <v>142</v>
       </c>
       <c r="B424" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
     </row>
     <row r="425" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B425" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
@@ -4031,12 +4073,12 @@
         <v>143</v>
       </c>
       <c r="B427" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
     </row>
     <row r="428" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B428" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
@@ -4044,12 +4086,12 @@
         <v>144</v>
       </c>
       <c r="B430" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="431" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B431" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
@@ -4057,12 +4099,12 @@
         <v>145</v>
       </c>
       <c r="B433" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
     </row>
     <row r="434" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B434" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
@@ -4070,12 +4112,12 @@
         <v>146</v>
       </c>
       <c r="B436" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
     </row>
     <row r="437" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B437" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
@@ -4083,12 +4125,12 @@
         <v>147</v>
       </c>
       <c r="B439" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="440" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B440" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
@@ -4096,12 +4138,12 @@
         <v>148</v>
       </c>
       <c r="B442" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="443" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B443" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
@@ -4109,12 +4151,12 @@
         <v>149</v>
       </c>
       <c r="B445" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
     <row r="446" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B446" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
@@ -4122,12 +4164,12 @@
         <v>150</v>
       </c>
       <c r="B448" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
     </row>
     <row r="449" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -4147,377 +4189,377 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
welcome message & cleanup
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -1,25 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28016"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Marshall/Desktop/PapaBot/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Admin" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Alliance" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Calendar" state="visible" r:id="rId6"/>
-    <sheet sheetId="4" name="Notes" state="visible" r:id="rId7"/>
-    <sheet sheetId="5" name="Jokes" state="visible" r:id="rId8"/>
-    <sheet sheetId="6" name="Roasts" state="visible" r:id="rId9"/>
+    <sheet name="Admin" sheetId="1" r:id="rId1"/>
+    <sheet name="Alliance" sheetId="2" r:id="rId2"/>
+    <sheet name="Calendar" sheetId="3" r:id="rId3"/>
+    <sheet name="Notes" sheetId="4" r:id="rId4"/>
+    <sheet name="Jokes" sheetId="5" r:id="rId5"/>
+    <sheet name="Roasts" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="449">
   <si>
     <t>allies</t>
   </si>
@@ -93,150 +106,153 @@
  - **!notes &lt;tag&gt; create** will add a new alliance to the list that we can add notes for.</t>
   </si>
   <si>
+    <t>2inpink 3instink</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>boricua</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>217</t>
+  </si>
+  <si>
+    <t>bubbarocker</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>copperpopo</t>
+  </si>
+  <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>creepingdeath</t>
+  </si>
+  <si>
+    <t>198</t>
+  </si>
+  <si>
+    <t>dirty diapers</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
+    <t>232</t>
+  </si>
+  <si>
+    <t>dracolatias</t>
+  </si>
+  <si>
+    <t>165</t>
+  </si>
+  <si>
+    <t>204</t>
+  </si>
+  <si>
+    <t>i n0mad i</t>
+  </si>
+  <si>
+    <t>218</t>
+  </si>
+  <si>
+    <t>ikandy1</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>199</t>
+  </si>
+  <si>
     <t>imothe1</t>
   </si>
   <si>
-    <t>161</t>
-  </si>
-  <si>
-    <t>101</t>
+    <t>178</t>
+  </si>
+  <si>
+    <t>kashmeoutside</t>
+  </si>
+  <si>
+    <t>182</t>
+  </si>
+  <si>
+    <t>korvvish</t>
+  </si>
+  <si>
+    <t>msbatman</t>
+  </si>
+  <si>
+    <t>203</t>
+  </si>
+  <si>
+    <t>nae blis</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>ocivv</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>papa marsh</t>
+  </si>
+  <si>
+    <t>peekaboo123</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>pratt11</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>rickys ruff riders</t>
+  </si>
+  <si>
+    <t>ru1900</t>
+  </si>
+  <si>
+    <t>216</t>
+  </si>
+  <si>
+    <t>sarcasticahole</t>
+  </si>
+  <si>
+    <t>shooty pants</t>
+  </si>
+  <si>
+    <t>teamgb</t>
+  </si>
+  <si>
+    <t>wrathavenger</t>
   </si>
   <si>
     <t>xmousecop</t>
   </si>
   <si>
-    <t>217</t>
-  </si>
-  <si>
-    <t>117</t>
-  </si>
-  <si>
-    <t>wrathavenger</t>
-  </si>
-  <si>
-    <t>178</t>
-  </si>
-  <si>
-    <t>118</t>
-  </si>
-  <si>
-    <t>teamgb</t>
-  </si>
-  <si>
-    <t>140</t>
-  </si>
-  <si>
-    <t>121</t>
-  </si>
-  <si>
-    <t>shooty pants</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>sarcasticahole</t>
-  </si>
-  <si>
-    <t>204</t>
-  </si>
-  <si>
-    <t>139</t>
-  </si>
-  <si>
-    <t>ru1900</t>
-  </si>
-  <si>
-    <t>216</t>
-  </si>
-  <si>
-    <t>rickys ruff riders</t>
-  </si>
-  <si>
-    <t>159</t>
-  </si>
-  <si>
-    <t>2inpink 3instink</t>
-  </si>
-  <si>
-    <t>pratt11</t>
-  </si>
-  <si>
-    <t>165</t>
-  </si>
-  <si>
-    <t>peekaboo123</t>
-  </si>
-  <si>
-    <t>177</t>
-  </si>
-  <si>
-    <t>papa marsh</t>
-  </si>
-  <si>
-    <t>199</t>
-  </si>
-  <si>
-    <t>ocivv</t>
-  </si>
-  <si>
-    <t>nae blis</t>
-  </si>
-  <si>
-    <t>86</t>
-  </si>
-  <si>
-    <t>202</t>
-  </si>
-  <si>
-    <t>msbatman</t>
-  </si>
-  <si>
-    <t>203</t>
-  </si>
-  <si>
-    <t>boricua</t>
-  </si>
-  <si>
-    <t>korvvish</t>
-  </si>
-  <si>
-    <t>232</t>
-  </si>
-  <si>
-    <t>kashmeoutside</t>
-  </si>
-  <si>
-    <t>182</t>
-  </si>
-  <si>
-    <t>198</t>
-  </si>
-  <si>
-    <t>ikandy1</t>
-  </si>
-  <si>
-    <t>i n0mad i</t>
-  </si>
-  <si>
-    <t>218</t>
-  </si>
-  <si>
-    <t>dracolatias</t>
-  </si>
-  <si>
-    <t>dirty diapers</t>
-  </si>
-  <si>
-    <t>creepingdeath</t>
-  </si>
-  <si>
-    <t>copperpopo</t>
-  </si>
-  <si>
-    <t>bubbarocker</t>
-  </si>
-  <si>
     <t>event</t>
   </si>
   <si>
@@ -1393,19 +1409,25 @@
   </si>
   <si>
     <t>are you always this stupid or is today a special occasion?</t>
+  </si>
+  <si>
+    <t>welcome</t>
+  </si>
+  <si>
+    <t>Please read through the #alliance-rules channel carefully for a summary on how we operate. Once your 'member' role is set, you'll be able to see the rest of the channels. If you have any questions, reach out to an officer at any time. To get familiar with some of the things PapaBot can do, type !help.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1431,10 +1453,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1750,71 +1772,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="8.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B7" s="2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B8" s="2" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1827,264 +1858,264 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
       <c r="C9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2094,28 +2125,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -2124,9 +2155,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B3">
         <v>22</v>
@@ -2135,9 +2166,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B4">
         <v>15</v>
@@ -2146,37 +2177,37 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
         <v>68</v>
       </c>
-      <c r="B6" t="s">
-        <v>67</v>
-      </c>
       <c r="C6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2186,13 +2217,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2202,1960 +2233,1960 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B449"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+    <sheetView workbookViewId="0">
       <selection activeCell="F232" sqref="F232"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>14</v>
       </c>
       <c r="B40" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>18</v>
       </c>
       <c r="B52" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>20</v>
       </c>
       <c r="B58" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>21</v>
       </c>
       <c r="B61" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>22</v>
       </c>
       <c r="B64" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>23</v>
       </c>
       <c r="B67" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>24</v>
       </c>
       <c r="B70" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>25</v>
       </c>
       <c r="B73" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>26</v>
       </c>
       <c r="B76" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>27</v>
       </c>
       <c r="B79" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>28</v>
       </c>
       <c r="B82" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>29</v>
       </c>
       <c r="B85" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>30</v>
       </c>
       <c r="B88" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>31</v>
       </c>
       <c r="B91" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>32</v>
       </c>
       <c r="B94" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>33</v>
       </c>
       <c r="B97" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>34</v>
       </c>
       <c r="B100" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>35</v>
       </c>
       <c r="B103" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>36</v>
       </c>
       <c r="B106" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>37</v>
       </c>
       <c r="B109" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>38</v>
       </c>
       <c r="B112" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>39</v>
       </c>
       <c r="B115" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>40</v>
       </c>
       <c r="B118" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>41</v>
       </c>
       <c r="B121" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>42</v>
       </c>
       <c r="B124" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>43</v>
       </c>
       <c r="B127" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>44</v>
       </c>
       <c r="B130" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>45</v>
       </c>
       <c r="B133" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>46</v>
       </c>
       <c r="B136" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>47</v>
       </c>
       <c r="B139" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>48</v>
       </c>
       <c r="B142" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>49</v>
       </c>
       <c r="B145" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>50</v>
       </c>
       <c r="B148" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>51</v>
       </c>
       <c r="B151" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>52</v>
       </c>
       <c r="B154" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>53</v>
       </c>
       <c r="B157" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>54</v>
       </c>
       <c r="B160" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>55</v>
       </c>
       <c r="B163" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>56</v>
       </c>
       <c r="B166" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>57</v>
       </c>
       <c r="B169" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>58</v>
       </c>
       <c r="B172" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>59</v>
       </c>
       <c r="B175" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>60</v>
       </c>
       <c r="B178" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>61</v>
       </c>
       <c r="B181" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>62</v>
       </c>
       <c r="B184" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>63</v>
       </c>
       <c r="B187" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B188" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>64</v>
       </c>
       <c r="B190" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B191" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>65</v>
       </c>
       <c r="B193" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B194" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>66</v>
       </c>
       <c r="B196" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B197" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>67</v>
       </c>
       <c r="B199" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B200" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>68</v>
       </c>
       <c r="B202" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B203" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>69</v>
       </c>
       <c r="B205" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B206" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>70</v>
       </c>
       <c r="B208" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B209" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>71</v>
       </c>
       <c r="B211" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B212" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>72</v>
       </c>
       <c r="B214" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B215" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>73</v>
       </c>
       <c r="B217" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B218" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>74</v>
       </c>
       <c r="B220" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B221" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>75</v>
       </c>
       <c r="B223" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B224" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>76</v>
       </c>
       <c r="B226" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B227" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>77</v>
       </c>
       <c r="B229" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B230" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>78</v>
       </c>
       <c r="B232" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B233" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>79</v>
       </c>
       <c r="B235" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B236" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>80</v>
       </c>
       <c r="B238" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B239" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>81</v>
       </c>
       <c r="B241" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B242" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>82</v>
       </c>
       <c r="B244" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B245" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>83</v>
       </c>
       <c r="B247" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B248" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>84</v>
       </c>
       <c r="B250" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B251" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>85</v>
       </c>
       <c r="B253" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B254" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>86</v>
       </c>
       <c r="B256" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B257" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>87</v>
       </c>
       <c r="B259" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B260" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>88</v>
       </c>
       <c r="B262" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B263" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>89</v>
       </c>
       <c r="B265" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="266" spans="2:2" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B266" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>90</v>
       </c>
       <c r="B268" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B269" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>91</v>
       </c>
       <c r="B271" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="272" spans="2:2" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B272" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>92</v>
       </c>
       <c r="B274" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B275" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>93</v>
       </c>
       <c r="B277" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B278" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>94</v>
       </c>
       <c r="B280" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="281" spans="2:2" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B281" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>95</v>
       </c>
       <c r="B283" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="284" spans="2:2" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B284" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>96</v>
       </c>
       <c r="B286" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="287" spans="2:2" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B287" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>97</v>
       </c>
       <c r="B289" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="290" spans="2:2" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B290" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>98</v>
       </c>
       <c r="B292" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="293" spans="2:2" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B293" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>99</v>
       </c>
       <c r="B295" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="296" spans="2:2" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B296" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>100</v>
       </c>
       <c r="B298" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="299" spans="2:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B299" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>101</v>
       </c>
       <c r="B301" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="302" spans="2:2" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B302" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>102</v>
       </c>
       <c r="B304" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="305" spans="2:2" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B305" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>103</v>
       </c>
       <c r="B307" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="308" spans="2:2" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B308" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>104</v>
       </c>
       <c r="B310" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="311" spans="2:2" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B311" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>105</v>
       </c>
       <c r="B313" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="314" spans="2:2" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B314" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>106</v>
       </c>
       <c r="B316" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="317" spans="2:2" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B317" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>107</v>
       </c>
       <c r="B319" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="320" spans="2:2" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B320" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>108</v>
       </c>
       <c r="B322" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="323" spans="2:2" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B323" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>109</v>
       </c>
       <c r="B325" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="326" spans="2:2" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B326" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>110</v>
       </c>
       <c r="B328" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="329" spans="2:2" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B329" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>111</v>
       </c>
       <c r="B331" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="332" spans="2:2" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B332" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>112</v>
       </c>
       <c r="B334" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="335" spans="2:2" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B335" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>113</v>
       </c>
       <c r="B337" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="338" spans="2:2" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B338" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>114</v>
       </c>
       <c r="B340" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="341" spans="2:2" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B341" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>115</v>
       </c>
       <c r="B343" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="344" spans="2:2" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B344" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>116</v>
       </c>
       <c r="B346" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="347" spans="2:2" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B347" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A349">
         <v>117</v>
       </c>
       <c r="B349" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="350" spans="2:2" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B350" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A352">
         <v>118</v>
       </c>
       <c r="B352" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="353" spans="2:2" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B353" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A355">
         <v>119</v>
       </c>
       <c r="B355" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="356" spans="2:2" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B356" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A358">
         <v>120</v>
       </c>
       <c r="B358" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="359" spans="2:2" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B359" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A361">
         <v>121</v>
       </c>
       <c r="B361" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="362" spans="2:2" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B362" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A364">
         <v>122</v>
       </c>
       <c r="B364" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="365" spans="2:2" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B365" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A367">
         <v>123</v>
       </c>
       <c r="B367" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="368" spans="2:2" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B368" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A370">
         <v>124</v>
       </c>
       <c r="B370" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="371" spans="2:2" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B371" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A373">
         <v>125</v>
       </c>
       <c r="B373" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="374" spans="2:2" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B374" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A376">
         <v>126</v>
       </c>
       <c r="B376" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="377" spans="2:2" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B377" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A379">
         <v>127</v>
       </c>
       <c r="B379" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="380" spans="2:2" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B380" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A382">
         <v>128</v>
       </c>
       <c r="B382" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="383" spans="2:2" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B383" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A385">
         <v>129</v>
       </c>
       <c r="B385" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="386" spans="2:2" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B386" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A388">
         <v>130</v>
       </c>
       <c r="B388" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="389" spans="2:2" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B389" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A391">
         <v>131</v>
       </c>
       <c r="B391" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="392" spans="2:2" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B392" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A394">
         <v>132</v>
       </c>
       <c r="B394" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="395" spans="2:2" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B395" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A397">
         <v>133</v>
       </c>
       <c r="B397" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="398" spans="2:2" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B398" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A400">
         <v>134</v>
       </c>
       <c r="B400" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="401" spans="2:2" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B401" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A403">
         <v>135</v>
       </c>
       <c r="B403" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="404" spans="2:2" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B404" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A406">
         <v>136</v>
       </c>
       <c r="B406" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="407" spans="2:2" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B407" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A409">
         <v>137</v>
       </c>
       <c r="B409" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="410" spans="2:2" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B410" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A412">
         <v>138</v>
       </c>
       <c r="B412" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="413" spans="2:2" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B413" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A415">
         <v>139</v>
       </c>
       <c r="B415" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="416" spans="2:2" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B416" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A418">
         <v>140</v>
       </c>
       <c r="B418" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="419" spans="2:2" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B419" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A421">
         <v>141</v>
       </c>
       <c r="B421" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="422" spans="2:2" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B422" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A424">
         <v>142</v>
       </c>
       <c r="B424" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="425" spans="2:2" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B425" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A427">
         <v>143</v>
       </c>
       <c r="B427" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="428" spans="2:2" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B428" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A430">
         <v>144</v>
       </c>
       <c r="B430" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="431" spans="2:2" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B431" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A433">
         <v>145</v>
       </c>
       <c r="B433" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="434" spans="2:2" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B434" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A436">
         <v>146</v>
       </c>
       <c r="B436" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="437" spans="2:2" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B437" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A439">
         <v>147</v>
       </c>
       <c r="B439" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="440" spans="2:2" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B440" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A442">
         <v>148</v>
       </c>
       <c r="B442" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="443" spans="2:2" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B443" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A445">
         <v>149</v>
       </c>
       <c r="B445" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="446" spans="2:2" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B446" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A448">
         <v>150</v>
       </c>
       <c r="B448" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="449" spans="2:2" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="449" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B449" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -4167,385 +4198,385 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A75"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+    <sheetView workbookViewId="0">
       <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
         <v>445</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
disconnect message, testing for member/user object, etc
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -19,18 +19,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="486">
   <si>
     <t>allies</t>
   </si>
   <si>
-    <t>Purple[808], Green[NFRC], and Red[REGAL]</t>
+    <t/>
   </si>
   <si>
     <t>plans</t>
-  </si>
-  <si>
-    <t>Defend against Blue. They will be sneak attacking! so heavy defenses on all choke points too.</t>
   </si>
   <si>
     <t>help</t>
@@ -103,90 +100,36 @@
     <t>2inpink 3instink</t>
   </si>
   <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>161</t>
-  </si>
-  <si>
     <t>boricua</t>
   </si>
   <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>217</t>
-  </si>
-  <si>
     <t>bubbarocker</t>
   </si>
   <si>
-    <t>139</t>
-  </si>
-  <si>
-    <t>86</t>
-  </si>
-  <si>
     <t>copperpopo</t>
   </si>
   <si>
-    <t>202</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
     <t>creepingdeath</t>
   </si>
   <si>
-    <t>198</t>
-  </si>
-  <si>
     <t>dirty diapers</t>
   </si>
   <si>
-    <t>159</t>
-  </si>
-  <si>
-    <t>232</t>
-  </si>
-  <si>
     <t>dracolatias</t>
   </si>
   <si>
-    <t>165</t>
-  </si>
-  <si>
-    <t>204</t>
-  </si>
-  <si>
     <t>i n0mad i</t>
   </si>
   <si>
-    <t>65</t>
-  </si>
-  <si>
     <t>ikandy1</t>
   </si>
   <si>
-    <t>177</t>
-  </si>
-  <si>
-    <t>199</t>
-  </si>
-  <si>
     <t>imothe1</t>
   </si>
   <si>
-    <t>178</t>
-  </si>
-  <si>
     <t>kashmeoutside</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>korvvish</t>
   </si>
   <si>
@@ -196,42 +139,24 @@
     <t>nae blis</t>
   </si>
   <si>
-    <t>140</t>
-  </si>
-  <si>
     <t>ocivv</t>
   </si>
   <si>
-    <t>117</t>
-  </si>
-  <si>
     <t>papa marsh</t>
   </si>
   <si>
     <t>peekaboo123</t>
   </si>
   <si>
-    <t>121</t>
-  </si>
-  <si>
     <t>pratt11</t>
   </si>
   <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>118</t>
-  </si>
-  <si>
     <t>rickys ruff riders</t>
   </si>
   <si>
     <t>ru1900</t>
   </si>
   <si>
-    <t>44</t>
-  </si>
-  <si>
     <t>sarcasticahole</t>
   </si>
   <si>
@@ -250,9 +175,6 @@
     <t>event</t>
   </si>
   <si>
-    <t>War 4: Final Reset</t>
-  </si>
-  <si>
     <t>month</t>
   </si>
   <si>
@@ -265,18 +187,12 @@
     <t>!5min</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
     <t>!1hour</t>
   </si>
   <si>
     <t>!1day</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>Q: What is the difference between your wife and your job?</t>
   </si>
   <si>
@@ -1465,76 +1381,139 @@
     <t>427515063507877888</t>
   </si>
   <si>
+    <t>mjm1976m</t>
+  </si>
+  <si>
     <t>117048304646225924</t>
   </si>
   <si>
+    <t>Boricua</t>
+  </si>
+  <si>
     <t>361739579977629697</t>
   </si>
   <si>
     <t>568608386791243799</t>
   </si>
   <si>
+    <t>Copperpopo</t>
+  </si>
+  <si>
     <t>621375239909015552</t>
   </si>
   <si>
     <t>621364830418239516</t>
   </si>
   <si>
+    <t>pilfer009</t>
+  </si>
+  <si>
     <t>623316383975079967</t>
   </si>
   <si>
+    <t>Draco</t>
+  </si>
+  <si>
     <t>484126152571617280</t>
   </si>
   <si>
+    <t>N0MADIC</t>
+  </si>
+  <si>
     <t>472627903104811019</t>
   </si>
   <si>
+    <t>IKANDY</t>
+  </si>
+  <si>
     <t>623622883201253411</t>
   </si>
   <si>
+    <t>imo the first</t>
+  </si>
+  <si>
     <t>463908810373857324</t>
   </si>
   <si>
+    <t>kash314</t>
+  </si>
+  <si>
     <t>395979105700413451</t>
   </si>
   <si>
+    <t>Korvvish</t>
+  </si>
+  <si>
     <t>478053793532084250</t>
   </si>
   <si>
     <t>409471590988906508</t>
   </si>
   <si>
+    <t>Nae’blis</t>
+  </si>
+  <si>
     <t>453762219042406401</t>
   </si>
   <si>
     <t>467426493912317953</t>
   </si>
   <si>
+    <t>PapaMarsh</t>
+  </si>
+  <si>
     <t>214042704357621760</t>
   </si>
   <si>
+    <t>dancingpotato</t>
+  </si>
+  <si>
     <t>370999241688219690</t>
   </si>
   <si>
+    <t>Pratt</t>
+  </si>
+  <si>
     <t>477018053133991937</t>
   </si>
   <si>
+    <t>Ricky</t>
+  </si>
+  <si>
     <t>621404757042659328</t>
   </si>
   <si>
+    <t>Ru</t>
+  </si>
+  <si>
     <t>535659584027754497</t>
   </si>
   <si>
+    <t>SarcasticAhole</t>
+  </si>
+  <si>
     <t>305697563175157760</t>
   </si>
   <si>
+    <t>shooty-pants</t>
+  </si>
+  <si>
     <t>428221019409350666</t>
   </si>
   <si>
+    <t>TeamGB</t>
+  </si>
+  <si>
     <t>246021971601522688</t>
   </si>
   <si>
+    <t>SilviuPOWER</t>
+  </si>
+  <si>
     <t>420761034941530113</t>
+  </si>
+  <si>
+    <t>mousecop</t>
   </si>
 </sst>
 </file>
@@ -1929,53 +1908,53 @@
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1995,274 +1974,127 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" t="s">
         <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" t="s">
         <v>33</v>
-      </c>
-      <c r="C21" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2272,7 +2104,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="B1" sqref="B1"/>
@@ -2280,60 +2112,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2370,1837 +2181,1837 @@
   <sheetData>
     <row r="1" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>185</v>
+        <v>157</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
-        <v>197</v>
+        <v>169</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>201</v>
+        <v>173</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>202</v>
+        <v>174</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>203</v>
+        <v>175</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>204</v>
+        <v>176</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>205</v>
+        <v>177</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>206</v>
+        <v>178</v>
       </c>
     </row>
     <row r="69" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>207</v>
+        <v>179</v>
       </c>
     </row>
     <row r="70" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>209</v>
+        <v>181</v>
       </c>
     </row>
     <row r="71" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
     </row>
     <row r="72" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
     </row>
     <row r="73" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>213</v>
+        <v>185</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
     </row>
     <row r="74" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
     </row>
     <row r="75" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
     </row>
     <row r="76" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
     </row>
     <row r="77" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
     </row>
     <row r="79" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
     </row>
     <row r="80" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>221</v>
+        <v>193</v>
       </c>
     </row>
     <row r="82" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>222</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>223</v>
+        <v>195</v>
       </c>
     </row>
     <row r="85" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
     </row>
     <row r="86" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
     </row>
     <row r="88" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>226</v>
+        <v>198</v>
       </c>
     </row>
     <row r="89" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>227</v>
+        <v>199</v>
       </c>
     </row>
     <row r="91" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>228</v>
+        <v>200</v>
       </c>
     </row>
     <row r="92" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
     </row>
     <row r="94" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
     </row>
     <row r="95" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>231</v>
+        <v>203</v>
       </c>
     </row>
     <row r="97" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>232</v>
+        <v>204</v>
       </c>
     </row>
     <row r="98" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
     </row>
     <row r="100" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>234</v>
+        <v>206</v>
       </c>
     </row>
     <row r="101" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>235</v>
+        <v>207</v>
       </c>
     </row>
     <row r="103" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>236</v>
+        <v>208</v>
       </c>
     </row>
     <row r="104" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>237</v>
+        <v>209</v>
       </c>
     </row>
     <row r="106" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
     </row>
     <row r="107" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
     </row>
     <row r="109" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
     </row>
     <row r="110" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
     </row>
     <row r="112" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
     </row>
     <row r="113" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="115" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="116" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
     </row>
     <row r="118" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
     </row>
     <row r="119" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
     </row>
     <row r="121" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
     </row>
     <row r="122" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>249</v>
+        <v>221</v>
       </c>
     </row>
     <row r="124" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>250</v>
+        <v>222</v>
       </c>
     </row>
     <row r="125" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
     </row>
     <row r="127" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
     </row>
     <row r="128" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
     </row>
     <row r="130" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>254</v>
+        <v>226</v>
       </c>
     </row>
     <row r="131" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>255</v>
+        <v>227</v>
       </c>
     </row>
     <row r="133" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
     </row>
     <row r="134" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>257</v>
+        <v>229</v>
       </c>
     </row>
     <row r="136" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>258</v>
+        <v>230</v>
       </c>
     </row>
     <row r="137" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
     </row>
     <row r="139" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
     </row>
     <row r="140" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
     </row>
     <row r="142" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
     </row>
     <row r="143" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
     </row>
     <row r="145" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
     </row>
     <row r="146" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
     </row>
     <row r="148" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>266</v>
+        <v>238</v>
       </c>
     </row>
     <row r="149" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>267</v>
+        <v>239</v>
       </c>
     </row>
     <row r="151" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
     </row>
     <row r="152" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
     </row>
     <row r="154" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
     </row>
     <row r="155" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>271</v>
+        <v>243</v>
       </c>
     </row>
     <row r="157" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>272</v>
+        <v>244</v>
       </c>
     </row>
     <row r="158" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>273</v>
+        <v>245</v>
       </c>
     </row>
     <row r="160" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>274</v>
+        <v>246</v>
       </c>
     </row>
     <row r="161" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="163" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>276</v>
+        <v>248</v>
       </c>
     </row>
     <row r="164" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
     <row r="166" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>278</v>
+        <v>250</v>
       </c>
     </row>
     <row r="167" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>279</v>
+        <v>251</v>
       </c>
     </row>
     <row r="169" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>280</v>
+        <v>252</v>
       </c>
     </row>
     <row r="170" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>281</v>
+        <v>253</v>
       </c>
     </row>
     <row r="172" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="173" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>283</v>
+        <v>255</v>
       </c>
     </row>
     <row r="175" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>284</v>
+        <v>256</v>
       </c>
     </row>
     <row r="176" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>285</v>
+        <v>257</v>
       </c>
     </row>
     <row r="178" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>286</v>
+        <v>258</v>
       </c>
     </row>
     <row r="179" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>287</v>
+        <v>259</v>
       </c>
     </row>
     <row r="181" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>288</v>
+        <v>260</v>
       </c>
     </row>
     <row r="182" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>289</v>
+        <v>261</v>
       </c>
     </row>
     <row r="184" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>290</v>
+        <v>262</v>
       </c>
     </row>
     <row r="185" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>291</v>
+        <v>263</v>
       </c>
     </row>
     <row r="187" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>292</v>
+        <v>264</v>
       </c>
     </row>
     <row r="188" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>293</v>
+        <v>265</v>
       </c>
     </row>
     <row r="190" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>294</v>
+        <v>266</v>
       </c>
     </row>
     <row r="191" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>295</v>
+        <v>267</v>
       </c>
     </row>
     <row r="193" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>296</v>
+        <v>268</v>
       </c>
     </row>
     <row r="194" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>297</v>
+        <v>269</v>
       </c>
     </row>
     <row r="196" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>298</v>
+        <v>270</v>
       </c>
     </row>
     <row r="197" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
     </row>
     <row r="199" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>300</v>
+        <v>272</v>
       </c>
     </row>
     <row r="200" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>301</v>
+        <v>273</v>
       </c>
     </row>
     <row r="202" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>302</v>
+        <v>274</v>
       </c>
     </row>
     <row r="203" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>303</v>
+        <v>275</v>
       </c>
     </row>
     <row r="205" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>304</v>
+        <v>276</v>
       </c>
     </row>
     <row r="206" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>305</v>
+        <v>277</v>
       </c>
     </row>
     <row r="208" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>306</v>
+        <v>278</v>
       </c>
     </row>
     <row r="209" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>307</v>
+        <v>279</v>
       </c>
     </row>
     <row r="211" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>308</v>
+        <v>280</v>
       </c>
     </row>
     <row r="212" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>309</v>
+        <v>281</v>
       </c>
     </row>
     <row r="214" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>310</v>
+        <v>282</v>
       </c>
     </row>
     <row r="215" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>311</v>
+        <v>283</v>
       </c>
     </row>
     <row r="217" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
     </row>
     <row r="218" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>313</v>
+        <v>285</v>
       </c>
     </row>
     <row r="220" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>314</v>
+        <v>286</v>
       </c>
     </row>
     <row r="221" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>315</v>
+        <v>287</v>
       </c>
     </row>
     <row r="223" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>316</v>
+        <v>288</v>
       </c>
     </row>
     <row r="224" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>317</v>
+        <v>289</v>
       </c>
     </row>
     <row r="226" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>318</v>
+        <v>290</v>
       </c>
     </row>
     <row r="227" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>319</v>
+        <v>291</v>
       </c>
     </row>
     <row r="229" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>320</v>
+        <v>292</v>
       </c>
     </row>
     <row r="230" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>321</v>
+        <v>293</v>
       </c>
     </row>
     <row r="232" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>322</v>
+        <v>294</v>
       </c>
     </row>
     <row r="233" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>323</v>
+        <v>295</v>
       </c>
     </row>
     <row r="235" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>324</v>
+        <v>296</v>
       </c>
     </row>
     <row r="236" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>325</v>
+        <v>297</v>
       </c>
     </row>
     <row r="238" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>326</v>
+        <v>298</v>
       </c>
     </row>
     <row r="239" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
-        <v>327</v>
+        <v>299</v>
       </c>
     </row>
     <row r="241" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>328</v>
+        <v>300</v>
       </c>
     </row>
     <row r="242" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>329</v>
+        <v>301</v>
       </c>
     </row>
     <row r="244" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
-        <v>330</v>
+        <v>302</v>
       </c>
     </row>
     <row r="245" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
-        <v>331</v>
+        <v>303</v>
       </c>
     </row>
     <row r="247" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>332</v>
+        <v>304</v>
       </c>
     </row>
     <row r="248" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>333</v>
+        <v>305</v>
       </c>
     </row>
     <row r="250" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>334</v>
+        <v>306</v>
       </c>
     </row>
     <row r="251" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>335</v>
+        <v>307</v>
       </c>
     </row>
     <row r="253" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>336</v>
+        <v>308</v>
       </c>
     </row>
     <row r="254" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>337</v>
+        <v>309</v>
       </c>
     </row>
     <row r="256" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
-        <v>338</v>
+        <v>310</v>
       </c>
     </row>
     <row r="257" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>339</v>
+        <v>311</v>
       </c>
     </row>
     <row r="259" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>340</v>
+        <v>312</v>
       </c>
     </row>
     <row r="260" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>341</v>
+        <v>313</v>
       </c>
     </row>
     <row r="262" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
-        <v>342</v>
+        <v>314</v>
       </c>
     </row>
     <row r="263" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>343</v>
+        <v>315</v>
       </c>
     </row>
     <row r="265" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>344</v>
+        <v>316</v>
       </c>
     </row>
     <row r="266" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>345</v>
+        <v>317</v>
       </c>
     </row>
     <row r="268" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>346</v>
+        <v>318</v>
       </c>
     </row>
     <row r="269" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>347</v>
+        <v>319</v>
       </c>
     </row>
     <row r="271" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>348</v>
+        <v>320</v>
       </c>
     </row>
     <row r="272" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>349</v>
+        <v>321</v>
       </c>
     </row>
     <row r="274" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
-        <v>350</v>
+        <v>322</v>
       </c>
     </row>
     <row r="275" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
-        <v>351</v>
+        <v>323</v>
       </c>
     </row>
     <row r="277" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>352</v>
+        <v>324</v>
       </c>
     </row>
     <row r="278" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>353</v>
+        <v>325</v>
       </c>
     </row>
     <row r="280" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>354</v>
+        <v>326</v>
       </c>
     </row>
     <row r="281" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>355</v>
+        <v>327</v>
       </c>
     </row>
     <row r="283" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>356</v>
+        <v>328</v>
       </c>
     </row>
     <row r="284" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>357</v>
+        <v>329</v>
       </c>
     </row>
     <row r="286" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>358</v>
+        <v>330</v>
       </c>
     </row>
     <row r="287" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>359</v>
+        <v>331</v>
       </c>
     </row>
     <row r="289" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>360</v>
+        <v>332</v>
       </c>
     </row>
     <row r="290" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>361</v>
+        <v>333</v>
       </c>
     </row>
     <row r="292" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>362</v>
+        <v>334</v>
       </c>
     </row>
     <row r="293" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>363</v>
+        <v>335</v>
       </c>
     </row>
     <row r="295" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
-        <v>364</v>
+        <v>336</v>
       </c>
     </row>
     <row r="296" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>365</v>
+        <v>337</v>
       </c>
     </row>
     <row r="298" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
     </row>
     <row r="299" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>367</v>
+        <v>339</v>
       </c>
     </row>
     <row r="301" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
-        <v>368</v>
+        <v>340</v>
       </c>
     </row>
     <row r="302" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
-        <v>369</v>
+        <v>341</v>
       </c>
     </row>
     <row r="304" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
-        <v>370</v>
+        <v>342</v>
       </c>
     </row>
     <row r="305" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
     </row>
     <row r="307" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
-        <v>372</v>
+        <v>344</v>
       </c>
     </row>
     <row r="308" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
-        <v>373</v>
+        <v>345</v>
       </c>
     </row>
     <row r="310" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
-        <v>374</v>
+        <v>346</v>
       </c>
     </row>
     <row r="311" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
-        <v>375</v>
+        <v>347</v>
       </c>
     </row>
     <row r="313" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
-        <v>376</v>
+        <v>348</v>
       </c>
     </row>
     <row r="314" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
-        <v>377</v>
+        <v>349</v>
       </c>
     </row>
     <row r="316" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>378</v>
+        <v>350</v>
       </c>
     </row>
     <row r="317" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>379</v>
+        <v>351</v>
       </c>
     </row>
     <row r="319" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
-        <v>380</v>
+        <v>352</v>
       </c>
     </row>
     <row r="320" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
-        <v>381</v>
+        <v>353</v>
       </c>
     </row>
     <row r="322" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
-        <v>382</v>
+        <v>354</v>
       </c>
     </row>
     <row r="323" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
-        <v>383</v>
+        <v>355</v>
       </c>
     </row>
     <row r="325" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
-        <v>384</v>
+        <v>356</v>
       </c>
     </row>
     <row r="326" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
-        <v>385</v>
+        <v>357</v>
       </c>
     </row>
     <row r="328" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
-        <v>386</v>
+        <v>358</v>
       </c>
     </row>
     <row r="329" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
-        <v>387</v>
+        <v>359</v>
       </c>
     </row>
     <row r="331" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
-        <v>388</v>
+        <v>360</v>
       </c>
     </row>
     <row r="332" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
-        <v>389</v>
+        <v>361</v>
       </c>
     </row>
     <row r="334" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
-        <v>390</v>
+        <v>362</v>
       </c>
     </row>
     <row r="335" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
-        <v>391</v>
+        <v>363</v>
       </c>
     </row>
     <row r="337" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
-        <v>392</v>
+        <v>364</v>
       </c>
     </row>
     <row r="338" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
-        <v>393</v>
+        <v>365</v>
       </c>
     </row>
     <row r="340" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
-        <v>394</v>
+        <v>366</v>
       </c>
     </row>
     <row r="341" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
-        <v>395</v>
+        <v>367</v>
       </c>
     </row>
     <row r="343" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
-        <v>396</v>
+        <v>368</v>
       </c>
     </row>
     <row r="344" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
-        <v>397</v>
+        <v>369</v>
       </c>
     </row>
     <row r="346" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
-        <v>398</v>
+        <v>370</v>
       </c>
     </row>
     <row r="347" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
-        <v>399</v>
+        <v>371</v>
       </c>
     </row>
     <row r="349" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
-        <v>400</v>
+        <v>372</v>
       </c>
     </row>
     <row r="350" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
-        <v>401</v>
+        <v>373</v>
       </c>
     </row>
     <row r="352" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
-        <v>402</v>
+        <v>374</v>
       </c>
     </row>
     <row r="353" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
-        <v>403</v>
+        <v>375</v>
       </c>
     </row>
     <row r="355" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
-        <v>404</v>
+        <v>376</v>
       </c>
     </row>
     <row r="356" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
-        <v>405</v>
+        <v>377</v>
       </c>
     </row>
     <row r="358" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
-        <v>406</v>
+        <v>378</v>
       </c>
     </row>
     <row r="359" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
-        <v>407</v>
+        <v>379</v>
       </c>
     </row>
     <row r="361" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
-        <v>408</v>
+        <v>380</v>
       </c>
     </row>
     <row r="362" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
-        <v>409</v>
+        <v>381</v>
       </c>
     </row>
     <row r="364" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
-        <v>410</v>
+        <v>382</v>
       </c>
     </row>
     <row r="365" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
-        <v>411</v>
+        <v>383</v>
       </c>
     </row>
     <row r="367" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
-        <v>412</v>
+        <v>384</v>
       </c>
     </row>
     <row r="368" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
-        <v>413</v>
+        <v>385</v>
       </c>
     </row>
     <row r="370" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
-        <v>414</v>
+        <v>386</v>
       </c>
     </row>
     <row r="371" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
-        <v>415</v>
+        <v>387</v>
       </c>
     </row>
     <row r="373" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
-        <v>416</v>
+        <v>388</v>
       </c>
     </row>
     <row r="374" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
-        <v>417</v>
+        <v>389</v>
       </c>
     </row>
     <row r="376" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
-        <v>418</v>
+        <v>390</v>
       </c>
     </row>
     <row r="377" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
-        <v>419</v>
+        <v>391</v>
       </c>
     </row>
     <row r="379" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
-        <v>420</v>
+        <v>392</v>
       </c>
     </row>
     <row r="380" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
-        <v>421</v>
+        <v>393</v>
       </c>
     </row>
     <row r="382" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
-        <v>422</v>
+        <v>394</v>
       </c>
     </row>
     <row r="383" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
-        <v>423</v>
+        <v>395</v>
       </c>
     </row>
     <row r="385" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
-        <v>424</v>
+        <v>396</v>
       </c>
     </row>
     <row r="386" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
-        <v>425</v>
+        <v>397</v>
       </c>
     </row>
     <row r="388" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
-        <v>426</v>
+        <v>398</v>
       </c>
     </row>
     <row r="389" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
-        <v>427</v>
+        <v>399</v>
       </c>
     </row>
     <row r="391" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
-        <v>428</v>
+        <v>400</v>
       </c>
     </row>
     <row r="392" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
-        <v>429</v>
+        <v>401</v>
       </c>
     </row>
     <row r="394" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
-        <v>430</v>
+        <v>402</v>
       </c>
     </row>
     <row r="395" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
-        <v>431</v>
+        <v>403</v>
       </c>
     </row>
     <row r="397" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
-        <v>432</v>
+        <v>404</v>
       </c>
     </row>
     <row r="398" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
-        <v>433</v>
+        <v>405</v>
       </c>
     </row>
     <row r="400" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
-        <v>434</v>
+        <v>406</v>
       </c>
     </row>
     <row r="401" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
-        <v>435</v>
+        <v>407</v>
       </c>
     </row>
     <row r="403" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
-        <v>436</v>
+        <v>408</v>
       </c>
     </row>
     <row r="404" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
-        <v>437</v>
+        <v>409</v>
       </c>
     </row>
     <row r="406" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
-        <v>438</v>
+        <v>410</v>
       </c>
     </row>
     <row r="407" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
-        <v>439</v>
+        <v>411</v>
       </c>
     </row>
     <row r="409" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
-        <v>440</v>
+        <v>412</v>
       </c>
     </row>
     <row r="410" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
-        <v>441</v>
+        <v>413</v>
       </c>
     </row>
     <row r="412" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
-        <v>442</v>
+        <v>414</v>
       </c>
     </row>
     <row r="413" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
-        <v>443</v>
+        <v>415</v>
       </c>
     </row>
     <row r="415" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
-        <v>444</v>
+        <v>416</v>
       </c>
     </row>
     <row r="416" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
-        <v>445</v>
+        <v>417</v>
       </c>
     </row>
     <row r="418" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
-        <v>446</v>
+        <v>418</v>
       </c>
     </row>
     <row r="419" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
-        <v>447</v>
+        <v>419</v>
       </c>
     </row>
     <row r="421" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
-        <v>448</v>
+        <v>420</v>
       </c>
     </row>
     <row r="422" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
-        <v>449</v>
+        <v>421</v>
       </c>
     </row>
     <row r="424" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
-        <v>450</v>
+        <v>422</v>
       </c>
     </row>
     <row r="425" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A425" s="1" t="s">
-        <v>451</v>
+        <v>423</v>
       </c>
     </row>
     <row r="427" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A427" s="1" t="s">
-        <v>452</v>
+        <v>424</v>
       </c>
     </row>
     <row r="428" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A428" s="1" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
     </row>
     <row r="430" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
     </row>
     <row r="431" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A431" s="1" t="s">
-        <v>455</v>
+        <v>427</v>
       </c>
     </row>
     <row r="433" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" s="1" t="s">
-        <v>456</v>
+        <v>428</v>
       </c>
     </row>
     <row r="434" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434" s="1" t="s">
-        <v>457</v>
+        <v>429</v>
       </c>
     </row>
     <row r="436" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436" s="1" t="s">
-        <v>458</v>
+        <v>430</v>
       </c>
     </row>
     <row r="437" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" s="1" t="s">
-        <v>459</v>
+        <v>431</v>
       </c>
     </row>
     <row r="439" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" s="1" t="s">
-        <v>460</v>
+        <v>432</v>
       </c>
     </row>
     <row r="440" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A440" s="1" t="s">
-        <v>461</v>
+        <v>433</v>
       </c>
     </row>
     <row r="442" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A442" s="1" t="s">
-        <v>462</v>
+        <v>434</v>
       </c>
     </row>
     <row r="443" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A443" s="1" t="s">
-        <v>463</v>
+        <v>435</v>
       </c>
     </row>
     <row r="445" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A445" s="1" t="s">
-        <v>464</v>
+        <v>436</v>
       </c>
     </row>
     <row r="446" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A446" s="1" t="s">
-        <v>465</v>
+        <v>437</v>
       </c>
     </row>
     <row r="448" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A448" s="1" t="s">
-        <v>466</v>
+        <v>438</v>
       </c>
     </row>
     <row r="449" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A449" s="1" t="s">
-        <v>467</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -4220,202 +4031,202 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>468</v>
+        <v>440</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>14</v>
+        <v>441</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>469</v>
+        <v>442</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>17</v>
+        <v>443</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>470</v>
+        <v>444</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>471</v>
+        <v>445</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>446</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>472</v>
+        <v>447</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>473</v>
+        <v>448</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>28</v>
+        <v>449</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>474</v>
+        <v>450</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>451</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>475</v>
+        <v>452</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>453</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>476</v>
+        <v>454</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>36</v>
+        <v>455</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>477</v>
+        <v>456</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>39</v>
+        <v>457</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>478</v>
+        <v>458</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>41</v>
+        <v>459</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>479</v>
+        <v>460</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>43</v>
+        <v>461</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>480</v>
+        <v>462</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>481</v>
+        <v>463</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>45</v>
+        <v>464</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>482</v>
+        <v>465</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>483</v>
+        <v>466</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>49</v>
+        <v>467</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>484</v>
+        <v>468</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>50</v>
+        <v>469</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>52</v>
+        <v>471</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>55</v>
+        <v>473</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>56</v>
+        <v>475</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>488</v>
+        <v>476</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>58</v>
+        <v>477</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>59</v>
+        <v>479</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>490</v>
+        <v>480</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>60</v>
+        <v>481</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>61</v>
+        <v>483</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>62</v>
+        <v>485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Discord UserID & username tracking
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Admin" state="visible" r:id="rId4"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="507">
   <si>
     <t>allies</t>
   </si>
@@ -1459,6 +1459,9 @@
     <t>kash314</t>
   </si>
   <si>
+    <t>20 Jan 2019 06:41:00 GMT</t>
+  </si>
+  <si>
     <t>395979105700413451</t>
   </si>
   <si>
@@ -1558,10 +1561,19 @@
     <t>262441739523063809</t>
   </si>
   <si>
+    <t>jimmylalao</t>
+  </si>
+  <si>
     <t>431633842634358794</t>
   </si>
   <si>
+    <t>Kamakrazy</t>
+  </si>
+  <si>
     <t>621354689501593620</t>
+  </si>
+  <si>
+    <t>PapaBot</t>
   </si>
   <si>
     <t>11 Sep 2019 14:48:17 GMT</t>
@@ -1937,9 +1949,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2016,7 +2028,7 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2156,7 +2168,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2206,7 +2218,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2220,9 +2232,9 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -4070,10 +4082,10 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -4176,28 +4188,31 @@
         <v>464</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>465</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>466</v>
       </c>
+      <c r="C11" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C12" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>25</v>
@@ -4205,18 +4220,18 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C14" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>27</v>
@@ -4224,112 +4239,121 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C16" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C21" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C24" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C25" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+      <c r="B26" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>500</v>
+        <v>502</v>
+      </c>
+      <c r="B27" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>501</v>
+        <v>504</v>
+      </c>
+      <c r="B28" t="s">
+        <v>505</v>
       </c>
       <c r="C28" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
do we even care about !status?
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="493">
   <si>
     <t>allies</t>
   </si>
@@ -1384,18 +1384,12 @@
     <t>mjm1976m</t>
   </si>
   <si>
-    <t>15 Sep 2019 17:46:38 GMT</t>
-  </si>
-  <si>
     <t>117048304646225924</t>
   </si>
   <si>
     <t>Boricua</t>
   </si>
   <si>
-    <t>06 Sep 2019 03:05:41 GMT</t>
-  </si>
-  <si>
     <t>361739579977629697</t>
   </si>
   <si>
@@ -1405,24 +1399,15 @@
     <t>Copperpopo</t>
   </si>
   <si>
-    <t>11 Sep 2019 14:51:28 GMT</t>
-  </si>
-  <si>
     <t>621375239909015552</t>
   </si>
   <si>
-    <t>11 Sep 2019 16:04:49 GMT</t>
-  </si>
-  <si>
     <t>621364830418239516</t>
   </si>
   <si>
     <t>pilfer009</t>
   </si>
   <si>
-    <t>11 Sep 2019 15:25:04 GMT</t>
-  </si>
-  <si>
     <t>623316383975079967</t>
   </si>
   <si>
@@ -1435,16 +1420,13 @@
     <t>N0MADIC</t>
   </si>
   <si>
-    <t>15 Sep 2019 17:26:19 GMT</t>
-  </si>
-  <si>
     <t>472627903104811019</t>
   </si>
   <si>
     <t>IKANDY</t>
   </si>
   <si>
-    <t>06 Sep 2019 02:34:36 GMT</t>
+    <t>25 Sep 2019 15:42:40 GMT</t>
   </si>
   <si>
     <t>623622883201253411</t>
@@ -1459,18 +1441,12 @@
     <t>kash314</t>
   </si>
   <si>
-    <t>20 Jan 2019 06:41:00 GMT</t>
-  </si>
-  <si>
     <t>395979105700413451</t>
   </si>
   <si>
     <t>Korvvish</t>
   </si>
   <si>
-    <t>17 Jan 2019 21:03:26 GMT</t>
-  </si>
-  <si>
     <t>478053793532084250</t>
   </si>
   <si>
@@ -1480,9 +1456,6 @@
     <t>Nae’blis</t>
   </si>
   <si>
-    <t>17 Jan 2019 21:12:35 GMT</t>
-  </si>
-  <si>
     <t>453762219042406401</t>
   </si>
   <si>
@@ -1492,9 +1465,6 @@
     <t>PapaMarsh</t>
   </si>
   <si>
-    <t>22 Mar 2019 14:26:29 GMT</t>
-  </si>
-  <si>
     <t>214042704357621760</t>
   </si>
   <si>
@@ -1525,9 +1495,6 @@
     <t>SarcasticAhole</t>
   </si>
   <si>
-    <t>18 Jan 2019 03:20:26 GMT</t>
-  </si>
-  <si>
     <t>305697563175157760</t>
   </si>
   <si>
@@ -1546,18 +1513,12 @@
     <t>SilviuPOWER</t>
   </si>
   <si>
-    <t>11 Sep 2019 19:30:56 GMT</t>
-  </si>
-  <si>
     <t>420761034941530113</t>
   </si>
   <si>
     <t>mousecop</t>
   </si>
   <si>
-    <t>16 Sep 2019 01:36:01 GMT</t>
-  </si>
-  <si>
     <t>262441739523063809</t>
   </si>
   <si>
@@ -1574,9 +1535,6 @@
   </si>
   <si>
     <t>PapaBot</t>
-  </si>
-  <si>
-    <t>11 Sep 2019 14:48:17 GMT</t>
   </si>
 </sst>
 </file>
@@ -4087,151 +4045,124 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>440</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>443</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>444</v>
-      </c>
-      <c r="C2" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>447</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>448</v>
-      </c>
-      <c r="C4" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>450</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="C6" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="C8" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C9" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>466</v>
-      </c>
-      <c r="C11" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>469</v>
-      </c>
-      <c r="C12" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>473</v>
-      </c>
-      <c r="C14" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>27</v>
@@ -4239,121 +4170,112 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="C16" t="s">
-        <v>478</v>
+        <v>456</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>485</v>
+        <v>475</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>487</v>
+        <v>477</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="C21" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>490</v>
+        <v>479</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>495</v>
-      </c>
-      <c r="C24" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>497</v>
+        <v>485</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>498</v>
-      </c>
-      <c r="C25" t="s">
-        <v>499</v>
+        <v>486</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>500</v>
+        <v>487</v>
       </c>
       <c r="B26" t="s">
-        <v>501</v>
+        <v>488</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>502</v>
+        <v>489</v>
       </c>
       <c r="B27" t="s">
-        <v>503</v>
+        <v>490</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>504</v>
+        <v>491</v>
       </c>
       <c r="B28" t="s">
-        <v>505</v>
+        <v>492</v>
       </c>
       <c r="C28" t="s">
-        <v>506</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove test message from backup
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="501">
   <si>
     <t>allies</t>
   </si>
@@ -1390,7 +1390,7 @@
     <t>Boricua</t>
   </si>
   <si>
-    <t>26 Sep 2019 00:50:26 GMT</t>
+    <t>26 Sep 2019 00:57:46 GMT</t>
   </si>
   <si>
     <t>361739579977629697</t>
@@ -1402,6 +1402,9 @@
     <t>Copperpopo</t>
   </si>
   <si>
+    <t>26 Sep 2019 00:52:16 GMT</t>
+  </si>
+  <si>
     <t>621375239909015552</t>
   </si>
   <si>
@@ -1429,7 +1432,7 @@
     <t>N0MADIC</t>
   </si>
   <si>
-    <t>25 Sep 2019 23:24:44 GMT</t>
+    <t>26 Sep 2019 01:03:06 GMT</t>
   </si>
   <si>
     <t>472627903104811019</t>
@@ -4101,91 +4104,91 @@
         <v>447</v>
       </c>
       <c r="C4" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C6" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C8" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C9" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C11" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>25</v>
@@ -4193,18 +4196,18 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C14" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>27</v>
@@ -4212,115 +4215,115 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C16" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C21" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B26" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B27" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B28" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C28" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
     </row>
   </sheetData>

</xml_diff>